<commit_message>
Section 2: Range Properties completed
</commit_message>
<xml_diff>
--- a/Ultimate Excel Programmer - VBA (Udemy) - Video Listing.xlsx
+++ b/Ultimate Excel Programmer - VBA (Udemy) - Video Listing.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="615" yWindow="225" windowWidth="22425" windowHeight="14745"/>
   </bookViews>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Unity Course Video Listing'!$3:$3</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1966,14 +1966,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J198"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="F1" s="34">
         <f>SUMIF(G4:G196, "&gt;0", C4:C196)</f>
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="G1" s="35">
         <f>+C197</f>
@@ -2009,7 +2009,7 @@
       </c>
       <c r="H1" s="36">
         <f>+F1/G1</f>
-        <v>5.0209205020920501E-2</v>
+        <v>8.3682008368200833E-2</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2455,7 +2455,7 @@
       </c>
       <c r="G17" s="41" t="str">
         <f>IF(COUNTA(G18:G27)=COUNTA(B18:B27), "COMPLETE", "")</f>
-        <v/>
+        <v>COMPLETE</v>
       </c>
       <c r="I17" s="9" t="str">
         <f t="shared" si="7"/>
@@ -2485,7 +2485,9 @@
         <f t="shared" si="6"/>
         <v>5.2998605299860529E-2</v>
       </c>
-      <c r="G18" s="30"/>
+      <c r="G18" s="30">
+        <v>42787</v>
+      </c>
       <c r="H18" s="30">
         <v>42787</v>
       </c>
@@ -2514,7 +2516,9 @@
         <f t="shared" si="6"/>
         <v>5.439330543933054E-2</v>
       </c>
-      <c r="G19" s="30"/>
+      <c r="G19" s="30">
+        <v>42787</v>
+      </c>
       <c r="H19" s="30">
         <v>42787</v>
       </c>
@@ -2543,7 +2547,9 @@
         <f t="shared" si="6"/>
         <v>5.5788005578800551E-2</v>
       </c>
-      <c r="G20" s="30"/>
+      <c r="G20" s="30">
+        <v>42787</v>
+      </c>
       <c r="H20" s="30">
         <v>42787</v>
       </c>
@@ -2572,7 +2578,9 @@
         <f t="shared" si="6"/>
         <v>5.7182705718270561E-2</v>
       </c>
-      <c r="G21" s="30"/>
+      <c r="G21" s="30">
+        <v>42787</v>
+      </c>
       <c r="H21" s="30">
         <v>42787</v>
       </c>
@@ -2601,7 +2609,9 @@
         <f t="shared" si="6"/>
         <v>5.997210599721059E-2</v>
       </c>
-      <c r="G22" s="30"/>
+      <c r="G22" s="30">
+        <v>42787</v>
+      </c>
       <c r="H22" s="30">
         <v>42787</v>
       </c>
@@ -2630,7 +2640,9 @@
         <f t="shared" si="6"/>
         <v>6.2761506276150611E-2</v>
       </c>
-      <c r="G23" s="30"/>
+      <c r="G23" s="30">
+        <v>42787</v>
+      </c>
       <c r="H23" s="30">
         <v>42787</v>
       </c>
@@ -2659,7 +2671,9 @@
         <f t="shared" si="6"/>
         <v>6.8340306834030667E-2</v>
       </c>
-      <c r="G24" s="30"/>
+      <c r="G24" s="30">
+        <v>42787</v>
+      </c>
       <c r="H24" s="30">
         <v>42787</v>
       </c>
@@ -2688,7 +2702,9 @@
         <f t="shared" si="6"/>
         <v>7.2524407252440706E-2</v>
       </c>
-      <c r="G25" s="30"/>
+      <c r="G25" s="30">
+        <v>42787</v>
+      </c>
       <c r="H25" s="30">
         <v>42787</v>
       </c>
@@ -2717,7 +2733,9 @@
         <f t="shared" si="6"/>
         <v>7.6708507670850745E-2</v>
       </c>
-      <c r="G26" s="30"/>
+      <c r="G26" s="30">
+        <v>42787</v>
+      </c>
       <c r="H26" s="30">
         <v>42787</v>
       </c>
@@ -2746,7 +2764,9 @@
         <f t="shared" si="6"/>
         <v>8.3682008368200819E-2</v>
       </c>
-      <c r="G27" s="30"/>
+      <c r="G27" s="30">
+        <v>42787</v>
+      </c>
       <c r="H27" s="30">
         <v>42787</v>
       </c>
@@ -7395,6 +7415,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:A219"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Section 3: Cells completed
</commit_message>
<xml_diff>
--- a/Ultimate Excel Programmer - VBA (Udemy) - Video Listing.xlsx
+++ b/Ultimate Excel Programmer - VBA (Udemy) - Video Listing.xlsx
@@ -1973,7 +1973,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="F1" s="34">
         <f>SUMIF(G4:G196, "&gt;0", C4:C196)</f>
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="G1" s="35">
         <f>+C197</f>
@@ -2009,7 +2009,7 @@
       </c>
       <c r="H1" s="36">
         <f>+F1/G1</f>
-        <v>8.3682008368200833E-2</v>
+        <v>0.10599721059972106</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2796,7 +2796,7 @@
       </c>
       <c r="G28" s="41" t="str">
         <f>IF(COUNTA(G29:G34)=COUNTA(B29:B34), "COMPLETE", "")</f>
-        <v/>
+        <v>COMPLETE</v>
       </c>
       <c r="I28" s="9" t="str">
         <f t="shared" si="7"/>
@@ -2826,7 +2826,9 @@
         <f t="shared" si="6"/>
         <v>8.7866108786610858E-2</v>
       </c>
-      <c r="G29" s="30"/>
+      <c r="G29" s="30">
+        <v>42787</v>
+      </c>
       <c r="H29" s="30">
         <v>42787</v>
       </c>
@@ -2855,7 +2857,9 @@
         <f t="shared" si="6"/>
         <v>8.9260808926080876E-2</v>
       </c>
-      <c r="G30" s="30"/>
+      <c r="G30" s="30">
+        <v>42787</v>
+      </c>
       <c r="H30" s="30">
         <v>42787</v>
       </c>
@@ -2884,7 +2888,9 @@
         <f t="shared" si="6"/>
         <v>9.2050209205020897E-2</v>
       </c>
-      <c r="G31" s="30"/>
+      <c r="G31" s="30">
+        <v>42787</v>
+      </c>
       <c r="H31" s="30">
         <v>42787</v>
       </c>
@@ -2913,7 +2919,9 @@
         <f t="shared" si="6"/>
         <v>9.4839609483960918E-2</v>
       </c>
-      <c r="G32" s="30"/>
+      <c r="G32" s="30">
+        <v>42787</v>
+      </c>
       <c r="H32" s="30">
         <v>42787</v>
       </c>
@@ -2942,7 +2950,9 @@
         <f t="shared" si="6"/>
         <v>9.9023709902370957E-2</v>
       </c>
-      <c r="G33" s="30"/>
+      <c r="G33" s="30">
+        <v>42787</v>
+      </c>
       <c r="H33" s="30">
         <v>42787</v>
       </c>
@@ -2971,7 +2981,9 @@
         <f t="shared" si="6"/>
         <v>0.10599721059972103</v>
       </c>
-      <c r="G34" s="30"/>
+      <c r="G34" s="30">
+        <v>42787</v>
+      </c>
       <c r="H34" s="30">
         <v>42787</v>
       </c>

</xml_diff>

<commit_message>
Section 4: Variables completed
</commit_message>
<xml_diff>
--- a/Ultimate Excel Programmer - VBA (Udemy) - Video Listing.xlsx
+++ b/Ultimate Excel Programmer - VBA (Udemy) - Video Listing.xlsx
@@ -1973,7 +1973,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="F1" s="34">
         <f>SUMIF(G4:G196, "&gt;0", C4:C196)</f>
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="G1" s="35">
         <f>+C197</f>
@@ -2009,7 +2009,7 @@
       </c>
       <c r="H1" s="36">
         <f>+F1/G1</f>
-        <v>0.10599721059972106</v>
+        <v>0.14783821478382148</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -3013,7 +3013,7 @@
       </c>
       <c r="G35" s="41" t="str">
         <f>IF(COUNTA(G36:G43)=COUNTA(B36:B43), "COMPLETE", "")</f>
-        <v/>
+        <v>COMPLETE</v>
       </c>
       <c r="I35" s="9" t="str">
         <f t="shared" si="7"/>
@@ -3043,7 +3043,9 @@
         <f t="shared" si="6"/>
         <v>0.11018131101813107</v>
       </c>
-      <c r="G36" s="30"/>
+      <c r="G36" s="30">
+        <v>42787</v>
+      </c>
       <c r="H36" s="30">
         <v>42787</v>
       </c>
@@ -3072,7 +3074,9 @@
         <f t="shared" si="6"/>
         <v>0.11436541143654111</v>
       </c>
-      <c r="G37" s="30"/>
+      <c r="G37" s="30">
+        <v>42787</v>
+      </c>
       <c r="H37" s="30">
         <v>42787</v>
       </c>
@@ -3101,7 +3105,9 @@
         <f t="shared" si="6"/>
         <v>0.12133891213389118</v>
       </c>
-      <c r="G38" s="30"/>
+      <c r="G38" s="30">
+        <v>42787</v>
+      </c>
       <c r="H38" s="30">
         <v>42787</v>
       </c>
@@ -3130,7 +3136,9 @@
         <f t="shared" si="6"/>
         <v>0.1241283124128312</v>
       </c>
-      <c r="G39" s="30"/>
+      <c r="G39" s="30">
+        <v>42787</v>
+      </c>
       <c r="H39" s="30">
         <v>42787</v>
       </c>
@@ -3159,7 +3167,9 @@
         <f t="shared" si="6"/>
         <v>0.12831241283124126</v>
       </c>
-      <c r="G40" s="30"/>
+      <c r="G40" s="30">
+        <v>42787</v>
+      </c>
       <c r="H40" s="30">
         <v>42787</v>
       </c>
@@ -3188,7 +3198,9 @@
         <f t="shared" si="6"/>
         <v>0.13110181311018129</v>
       </c>
-      <c r="G41" s="30"/>
+      <c r="G41" s="30">
+        <v>42787</v>
+      </c>
       <c r="H41" s="30">
         <v>42787</v>
       </c>
@@ -3217,7 +3229,9 @@
         <f t="shared" si="6"/>
         <v>0.14086471408647139</v>
       </c>
-      <c r="G42" s="30"/>
+      <c r="G42" s="30">
+        <v>42787</v>
+      </c>
       <c r="H42" s="30">
         <v>42787</v>
       </c>
@@ -3246,7 +3260,9 @@
         <f t="shared" si="6"/>
         <v>0.14783821478382145</v>
       </c>
-      <c r="G43" s="30"/>
+      <c r="G43" s="30">
+        <v>42787</v>
+      </c>
       <c r="H43" s="30">
         <v>42787</v>
       </c>

</xml_diff>

<commit_message>
Section 5: Toolbars and Menus completed
</commit_message>
<xml_diff>
--- a/Ultimate Excel Programmer - VBA (Udemy) - Video Listing.xlsx
+++ b/Ultimate Excel Programmer - VBA (Udemy) - Video Listing.xlsx
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="250">
   <si>
     <t>VIDEO NAME</t>
   </si>
@@ -1124,6 +1124,12 @@
   </si>
   <si>
     <t>165. Userform Report with Filters - Part 2   6:03</t>
+  </si>
+  <si>
+    <t>131. Compliance check part 2   9:50</t>
+  </si>
+  <si>
+    <t>130. Compliance Checker for your Forms or Quizzes Part 1   3:36</t>
   </si>
 </sst>
 </file>
@@ -1972,8 +1978,8 @@
   <dimension ref="A1:J198"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G45" sqref="G45"/>
+      <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2001,15 +2007,15 @@
       </c>
       <c r="F1" s="34">
         <f>SUMIF(G4:G196, "&gt;0", C4:C196)</f>
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="G1" s="35">
         <f>+C197</f>
-        <v>717</v>
+        <v>687</v>
       </c>
       <c r="H1" s="36">
         <f>+F1/G1</f>
-        <v>0.14783821478382148</v>
+        <v>0.20378457059679767</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2020,7 +2026,7 @@
       <c r="C2" s="4"/>
       <c r="G2" s="38">
         <f>+G1/60</f>
-        <v>11.95</v>
+        <v>11.45</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="45.75" thickBot="1">
@@ -2080,7 +2086,7 @@
       </c>
       <c r="F5" s="15">
         <f>F4+(C5/$C$197)</f>
-        <v>1.6736401673640166E-2</v>
+        <v>1.7467248908296942E-2</v>
       </c>
       <c r="G5" s="30">
         <v>42722</v>
@@ -2111,7 +2117,7 @@
       </c>
       <c r="F6" s="15">
         <f t="shared" ref="F6" si="3">F5+(C6/$C$197)</f>
-        <v>1.9525801952580194E-2</v>
+        <v>2.0378457059679767E-2</v>
       </c>
       <c r="G6" s="30">
         <v>42724</v>
@@ -2142,7 +2148,7 @@
       </c>
       <c r="F7" s="15">
         <f>F6+(C7/$C$197)</f>
-        <v>2.2315202231520222E-2</v>
+        <v>2.3289665211062592E-2</v>
       </c>
       <c r="G7" s="30">
         <v>42724</v>
@@ -2173,7 +2179,7 @@
       </c>
       <c r="F8" s="15">
         <f t="shared" ref="F8:F71" si="6">F7+(C8/$C$197)</f>
-        <v>2.6499302649930265E-2</v>
+        <v>2.7656477438136828E-2</v>
       </c>
       <c r="G8" s="30">
         <v>42724</v>
@@ -2204,7 +2210,7 @@
       </c>
       <c r="F9" s="15">
         <f t="shared" si="6"/>
-        <v>2.7894002789400279E-2</v>
+        <v>2.9112081513828238E-2</v>
       </c>
       <c r="G9" s="30">
         <v>42724</v>
@@ -2235,7 +2241,7 @@
       </c>
       <c r="F10" s="15">
         <f t="shared" si="6"/>
-        <v>3.0683403068340307E-2</v>
+        <v>3.2023289665211063E-2</v>
       </c>
       <c r="G10" s="30">
         <v>42724</v>
@@ -2266,7 +2272,7 @@
       </c>
       <c r="F11" s="15">
         <f t="shared" si="6"/>
-        <v>3.2078103207810321E-2</v>
+        <v>3.3478893740902474E-2</v>
       </c>
       <c r="G11" s="30">
         <v>42724</v>
@@ -2297,7 +2303,7 @@
       </c>
       <c r="F12" s="15">
         <f t="shared" si="6"/>
-        <v>3.4867503486750349E-2</v>
+        <v>3.6390101892285295E-2</v>
       </c>
       <c r="G12" s="30">
         <v>42724</v>
@@ -2328,7 +2334,7 @@
       </c>
       <c r="F13" s="15">
         <f t="shared" si="6"/>
-        <v>3.7656903765690378E-2</v>
+        <v>3.9301310043668117E-2</v>
       </c>
       <c r="G13" s="30">
         <v>42724</v>
@@ -2359,7 +2365,7 @@
       </c>
       <c r="F14" s="15">
         <f t="shared" si="6"/>
-        <v>4.0446304044630406E-2</v>
+        <v>4.2212518195050938E-2</v>
       </c>
       <c r="G14" s="30">
         <v>42724</v>
@@ -2390,7 +2396,7 @@
       </c>
       <c r="F15" s="15">
         <f t="shared" si="6"/>
-        <v>4.3235704323570434E-2</v>
+        <v>4.512372634643376E-2</v>
       </c>
       <c r="G15" s="30">
         <v>42724</v>
@@ -2421,7 +2427,7 @@
       </c>
       <c r="F16" s="15">
         <f t="shared" si="6"/>
-        <v>5.0209205020920501E-2</v>
+        <v>5.240174672489082E-2</v>
       </c>
       <c r="G16" s="30">
         <v>42724</v>
@@ -2451,7 +2457,7 @@
       <c r="E17" s="27"/>
       <c r="F17" s="29">
         <f t="shared" si="6"/>
-        <v>5.0209205020920501E-2</v>
+        <v>5.240174672489082E-2</v>
       </c>
       <c r="G17" s="41" t="str">
         <f>IF(COUNTA(G18:G27)=COUNTA(B18:B27), "COMPLETE", "")</f>
@@ -2483,7 +2489,7 @@
       </c>
       <c r="F18" s="15">
         <f t="shared" si="6"/>
-        <v>5.2998605299860529E-2</v>
+        <v>5.5312954876273641E-2</v>
       </c>
       <c r="G18" s="30">
         <v>42787</v>
@@ -2514,7 +2520,7 @@
       </c>
       <c r="F19" s="15">
         <f t="shared" si="6"/>
-        <v>5.439330543933054E-2</v>
+        <v>5.6768558951965052E-2</v>
       </c>
       <c r="G19" s="30">
         <v>42787</v>
@@ -2545,7 +2551,7 @@
       </c>
       <c r="F20" s="15">
         <f t="shared" si="6"/>
-        <v>5.5788005578800551E-2</v>
+        <v>5.8224163027656463E-2</v>
       </c>
       <c r="G20" s="30">
         <v>42787</v>
@@ -2576,7 +2582,7 @@
       </c>
       <c r="F21" s="15">
         <f t="shared" si="6"/>
-        <v>5.7182705718270561E-2</v>
+        <v>5.9679767103347874E-2</v>
       </c>
       <c r="G21" s="30">
         <v>42787</v>
@@ -2607,7 +2613,7 @@
       </c>
       <c r="F22" s="15">
         <f t="shared" si="6"/>
-        <v>5.997210599721059E-2</v>
+        <v>6.2590975254730702E-2</v>
       </c>
       <c r="G22" s="30">
         <v>42787</v>
@@ -2638,7 +2644,7 @@
       </c>
       <c r="F23" s="15">
         <f t="shared" si="6"/>
-        <v>6.2761506276150611E-2</v>
+        <v>6.5502183406113523E-2</v>
       </c>
       <c r="G23" s="30">
         <v>42787</v>
@@ -2669,7 +2675,7 @@
       </c>
       <c r="F24" s="15">
         <f t="shared" si="6"/>
-        <v>6.8340306834030667E-2</v>
+        <v>7.1324599708879166E-2</v>
       </c>
       <c r="G24" s="30">
         <v>42787</v>
@@ -2700,7 +2706,7 @@
       </c>
       <c r="F25" s="15">
         <f t="shared" si="6"/>
-        <v>7.2524407252440706E-2</v>
+        <v>7.5691411935953398E-2</v>
       </c>
       <c r="G25" s="30">
         <v>42787</v>
@@ -2731,7 +2737,7 @@
       </c>
       <c r="F26" s="15">
         <f t="shared" si="6"/>
-        <v>7.6708507670850745E-2</v>
+        <v>8.005822416302763E-2</v>
       </c>
       <c r="G26" s="30">
         <v>42787</v>
@@ -2762,7 +2768,7 @@
       </c>
       <c r="F27" s="15">
         <f t="shared" si="6"/>
-        <v>8.3682008368200819E-2</v>
+        <v>8.7336244541484684E-2</v>
       </c>
       <c r="G27" s="30">
         <v>42787</v>
@@ -2792,7 +2798,7 @@
       <c r="E28" s="27"/>
       <c r="F28" s="29">
         <f t="shared" si="6"/>
-        <v>8.3682008368200819E-2</v>
+        <v>8.7336244541484684E-2</v>
       </c>
       <c r="G28" s="41" t="str">
         <f>IF(COUNTA(G29:G34)=COUNTA(B29:B34), "COMPLETE", "")</f>
@@ -2824,7 +2830,7 @@
       </c>
       <c r="F29" s="15">
         <f t="shared" si="6"/>
-        <v>8.7866108786610858E-2</v>
+        <v>9.1703056768558916E-2</v>
       </c>
       <c r="G29" s="30">
         <v>42787</v>
@@ -2855,7 +2861,7 @@
       </c>
       <c r="F30" s="15">
         <f t="shared" si="6"/>
-        <v>8.9260808926080876E-2</v>
+        <v>9.3158660844250327E-2</v>
       </c>
       <c r="G30" s="30">
         <v>42787</v>
@@ -2886,7 +2892,7 @@
       </c>
       <c r="F31" s="15">
         <f t="shared" si="6"/>
-        <v>9.2050209205020897E-2</v>
+        <v>9.6069868995633148E-2</v>
       </c>
       <c r="G31" s="30">
         <v>42787</v>
@@ -2917,7 +2923,7 @@
       </c>
       <c r="F32" s="15">
         <f t="shared" si="6"/>
-        <v>9.4839609483960918E-2</v>
+        <v>9.8981077147015969E-2</v>
       </c>
       <c r="G32" s="30">
         <v>42787</v>
@@ -2948,7 +2954,7 @@
       </c>
       <c r="F33" s="15">
         <f t="shared" si="6"/>
-        <v>9.9023709902370957E-2</v>
+        <v>0.1033478893740902</v>
       </c>
       <c r="G33" s="30">
         <v>42787</v>
@@ -2979,7 +2985,7 @@
       </c>
       <c r="F34" s="15">
         <f t="shared" si="6"/>
-        <v>0.10599721059972103</v>
+        <v>0.11062590975254726</v>
       </c>
       <c r="G34" s="30">
         <v>42787</v>
@@ -3009,7 +3015,7 @@
       <c r="E35" s="27"/>
       <c r="F35" s="29">
         <f t="shared" si="6"/>
-        <v>0.10599721059972103</v>
+        <v>0.11062590975254726</v>
       </c>
       <c r="G35" s="41" t="str">
         <f>IF(COUNTA(G36:G43)=COUNTA(B36:B43), "COMPLETE", "")</f>
@@ -3041,7 +3047,7 @@
       </c>
       <c r="F36" s="15">
         <f t="shared" si="6"/>
-        <v>0.11018131101813107</v>
+        <v>0.11499272197962149</v>
       </c>
       <c r="G36" s="30">
         <v>42787</v>
@@ -3072,7 +3078,7 @@
       </c>
       <c r="F37" s="15">
         <f t="shared" si="6"/>
-        <v>0.11436541143654111</v>
+        <v>0.11935953420669572</v>
       </c>
       <c r="G37" s="30">
         <v>42787</v>
@@ -3103,7 +3109,7 @@
       </c>
       <c r="F38" s="15">
         <f t="shared" si="6"/>
-        <v>0.12133891213389118</v>
+        <v>0.12663755458515277</v>
       </c>
       <c r="G38" s="30">
         <v>42787</v>
@@ -3134,7 +3140,7 @@
       </c>
       <c r="F39" s="15">
         <f t="shared" si="6"/>
-        <v>0.1241283124128312</v>
+        <v>0.12954876273653559</v>
       </c>
       <c r="G39" s="30">
         <v>42787</v>
@@ -3165,7 +3171,7 @@
       </c>
       <c r="F40" s="15">
         <f t="shared" si="6"/>
-        <v>0.12831241283124126</v>
+        <v>0.13391557496360984</v>
       </c>
       <c r="G40" s="30">
         <v>42787</v>
@@ -3196,7 +3202,7 @@
       </c>
       <c r="F41" s="15">
         <f t="shared" si="6"/>
-        <v>0.13110181311018129</v>
+        <v>0.13682678311499266</v>
       </c>
       <c r="G41" s="30">
         <v>42787</v>
@@ -3227,7 +3233,7 @@
       </c>
       <c r="F42" s="15">
         <f t="shared" si="6"/>
-        <v>0.14086471408647139</v>
+        <v>0.14701601164483255</v>
       </c>
       <c r="G42" s="30">
         <v>42787</v>
@@ -3258,7 +3264,7 @@
       </c>
       <c r="F43" s="15">
         <f t="shared" si="6"/>
-        <v>0.14783821478382145</v>
+        <v>0.15429403202328962</v>
       </c>
       <c r="G43" s="30">
         <v>42787</v>
@@ -3288,11 +3294,11 @@
       <c r="E44" s="27"/>
       <c r="F44" s="29">
         <f t="shared" si="6"/>
-        <v>0.14783821478382145</v>
+        <v>0.15429403202328962</v>
       </c>
       <c r="G44" s="41" t="str">
         <f>IF(COUNTA(G45:G53)=COUNTA(B45:B53), "COMPLETE", "")</f>
-        <v/>
+        <v>COMPLETE</v>
       </c>
       <c r="I44" s="9" t="str">
         <f t="shared" si="7"/>
@@ -3320,10 +3326,14 @@
       </c>
       <c r="F45" s="15">
         <f t="shared" si="6"/>
-        <v>0.15062761506276148</v>
-      </c>
-      <c r="G45" s="30"/>
-      <c r="H45" s="30"/>
+        <v>0.15720524017467244</v>
+      </c>
+      <c r="G45" s="30">
+        <v>42788</v>
+      </c>
+      <c r="H45" s="30">
+        <v>42788</v>
+      </c>
       <c r="I45" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3347,10 +3357,14 @@
       </c>
       <c r="F46" s="15">
         <f t="shared" si="6"/>
-        <v>0.15760111576011154</v>
-      </c>
-      <c r="G46" s="30"/>
-      <c r="H46" s="30"/>
+        <v>0.16448326055312951</v>
+      </c>
+      <c r="G46" s="30">
+        <v>42788</v>
+      </c>
+      <c r="H46" s="30">
+        <v>42788</v>
+      </c>
       <c r="I46" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3374,10 +3388,14 @@
       </c>
       <c r="F47" s="15">
         <f t="shared" si="6"/>
-        <v>0.16039051603905158</v>
-      </c>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
+        <v>0.16739446870451233</v>
+      </c>
+      <c r="G47" s="30">
+        <v>42788</v>
+      </c>
+      <c r="H47" s="30">
+        <v>42788</v>
+      </c>
       <c r="I47" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3401,10 +3419,14 @@
       </c>
       <c r="F48" s="15">
         <f t="shared" si="6"/>
-        <v>0.17154811715481169</v>
-      </c>
-      <c r="G48" s="30"/>
-      <c r="H48" s="30"/>
+        <v>0.17903930131004361</v>
+      </c>
+      <c r="G48" s="30">
+        <v>42788</v>
+      </c>
+      <c r="H48" s="30">
+        <v>42788</v>
+      </c>
       <c r="I48" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3428,10 +3450,14 @@
       </c>
       <c r="F49" s="15">
         <f t="shared" si="6"/>
-        <v>0.17712691771269173</v>
-      </c>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
+        <v>0.18486171761280926</v>
+      </c>
+      <c r="G49" s="30">
+        <v>42788</v>
+      </c>
+      <c r="H49" s="30">
+        <v>42788</v>
+      </c>
       <c r="I49" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3455,10 +3481,14 @@
       </c>
       <c r="F50" s="15">
         <f t="shared" si="6"/>
-        <v>0.17852161785216175</v>
-      </c>
-      <c r="G50" s="30"/>
-      <c r="H50" s="30"/>
+        <v>0.18631732168850068</v>
+      </c>
+      <c r="G50" s="30">
+        <v>42788</v>
+      </c>
+      <c r="H50" s="30">
+        <v>42788</v>
+      </c>
       <c r="I50" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3482,10 +3512,14 @@
       </c>
       <c r="F51" s="15">
         <f t="shared" si="6"/>
-        <v>0.18549511854951181</v>
-      </c>
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
+        <v>0.19359534206695775</v>
+      </c>
+      <c r="G51" s="30">
+        <v>42788</v>
+      </c>
+      <c r="H51" s="30">
+        <v>42788</v>
+      </c>
       <c r="I51" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3509,10 +3543,14 @@
       </c>
       <c r="F52" s="15">
         <f t="shared" si="6"/>
-        <v>0.18828451882845185</v>
-      </c>
-      <c r="G52" s="30"/>
-      <c r="H52" s="30"/>
+        <v>0.19650655021834057</v>
+      </c>
+      <c r="G52" s="30">
+        <v>42788</v>
+      </c>
+      <c r="H52" s="30">
+        <v>42788</v>
+      </c>
       <c r="I52" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3536,10 +3574,14 @@
       </c>
       <c r="F53" s="15">
         <f t="shared" si="6"/>
-        <v>0.19525801952580191</v>
-      </c>
-      <c r="G53" s="30"/>
-      <c r="H53" s="30"/>
+        <v>0.20378457059679764</v>
+      </c>
+      <c r="G53" s="30">
+        <v>42788</v>
+      </c>
+      <c r="H53" s="30">
+        <v>42788</v>
+      </c>
       <c r="I53" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3562,7 +3604,7 @@
       <c r="E54" s="27"/>
       <c r="F54" s="29">
         <f t="shared" si="6"/>
-        <v>0.19525801952580191</v>
+        <v>0.20378457059679764</v>
       </c>
       <c r="G54" s="41" t="str">
         <f>IF(COUNTA(G55:G76)=COUNTA(B55:B76), "COMPLETE", "")</f>
@@ -3594,10 +3636,12 @@
       </c>
       <c r="F55" s="15">
         <f t="shared" si="6"/>
-        <v>0.19944211994421196</v>
+        <v>0.20815138282387188</v>
       </c>
       <c r="G55" s="30"/>
-      <c r="H55" s="30"/>
+      <c r="H55" s="30">
+        <v>42788</v>
+      </c>
       <c r="I55" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3621,10 +3665,12 @@
       </c>
       <c r="F56" s="15">
         <f t="shared" si="6"/>
-        <v>0.20362622036262201</v>
+        <v>0.21251819505094613</v>
       </c>
       <c r="G56" s="30"/>
-      <c r="H56" s="30"/>
+      <c r="H56" s="30">
+        <v>42788</v>
+      </c>
       <c r="I56" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3648,10 +3694,12 @@
       </c>
       <c r="F57" s="15">
         <f t="shared" si="6"/>
-        <v>0.20502092050209203</v>
+        <v>0.21397379912663755</v>
       </c>
       <c r="G57" s="30"/>
-      <c r="H57" s="30"/>
+      <c r="H57" s="30">
+        <v>42788</v>
+      </c>
       <c r="I57" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3675,10 +3723,12 @@
       </c>
       <c r="F58" s="15">
         <f t="shared" si="6"/>
-        <v>0.21059972105997207</v>
+        <v>0.2197962154294032</v>
       </c>
       <c r="G58" s="30"/>
-      <c r="H58" s="30"/>
+      <c r="H58" s="30">
+        <v>42788</v>
+      </c>
       <c r="I58" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3702,10 +3752,12 @@
       </c>
       <c r="F59" s="15">
         <f t="shared" si="6"/>
-        <v>0.21896792189679215</v>
+        <v>0.22852983988355166</v>
       </c>
       <c r="G59" s="30"/>
-      <c r="H59" s="30"/>
+      <c r="H59" s="30">
+        <v>42788</v>
+      </c>
       <c r="I59" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3729,10 +3781,12 @@
       </c>
       <c r="F60" s="15">
         <f t="shared" si="6"/>
-        <v>0.22454672245467219</v>
+        <v>0.2343522561863173</v>
       </c>
       <c r="G60" s="30"/>
-      <c r="H60" s="30"/>
+      <c r="H60" s="30">
+        <v>42788</v>
+      </c>
       <c r="I60" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3756,10 +3810,12 @@
       </c>
       <c r="F61" s="15">
         <f t="shared" si="6"/>
-        <v>0.22873082287308225</v>
+        <v>0.23871906841339155</v>
       </c>
       <c r="G61" s="30"/>
-      <c r="H61" s="30"/>
+      <c r="H61" s="30">
+        <v>42788</v>
+      </c>
       <c r="I61" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3783,17 +3839,19 @@
       </c>
       <c r="F62" s="15">
         <f t="shared" si="6"/>
-        <v>0.23012552301255226</v>
+        <v>0.24017467248908297</v>
       </c>
       <c r="G62" s="30"/>
-      <c r="H62" s="30"/>
-      <c r="I62" s="9" t="str">
+      <c r="H62" s="30">
+        <v>42788</v>
+      </c>
+      <c r="I62" s="9">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J62" s="38" t="str">
+        <v>59</v>
+      </c>
+      <c r="J62" s="38">
         <f t="shared" si="8"/>
-        <v/>
+        <v>0.98333333333333328</v>
       </c>
     </row>
     <row r="63" spans="1:10" outlineLevel="1">
@@ -3810,10 +3868,12 @@
       </c>
       <c r="F63" s="15">
         <f t="shared" si="6"/>
-        <v>0.23430962343096232</v>
+        <v>0.24454148471615722</v>
       </c>
       <c r="G63" s="30"/>
-      <c r="H63" s="30"/>
+      <c r="H63" s="30">
+        <v>42790</v>
+      </c>
       <c r="I63" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3837,10 +3897,12 @@
       </c>
       <c r="F64" s="15">
         <f t="shared" si="6"/>
-        <v>0.23570432357043233</v>
+        <v>0.24599708879184864</v>
       </c>
       <c r="G64" s="30"/>
-      <c r="H64" s="30"/>
+      <c r="H64" s="30">
+        <v>42790</v>
+      </c>
       <c r="I64" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3864,10 +3926,12 @@
       </c>
       <c r="F65" s="15">
         <f t="shared" si="6"/>
-        <v>0.23709902370990235</v>
+        <v>0.24745269286754007</v>
       </c>
       <c r="G65" s="30"/>
-      <c r="H65" s="30"/>
+      <c r="H65" s="30">
+        <v>42790</v>
+      </c>
       <c r="I65" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3891,10 +3955,12 @@
       </c>
       <c r="F66" s="15">
         <f t="shared" si="6"/>
-        <v>0.23988842398884239</v>
+        <v>0.25036390101892292</v>
       </c>
       <c r="G66" s="30"/>
-      <c r="H66" s="30"/>
+      <c r="H66" s="30">
+        <v>42790</v>
+      </c>
       <c r="I66" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3918,10 +3984,12 @@
       </c>
       <c r="F67" s="15">
         <f t="shared" si="6"/>
-        <v>0.24267782426778242</v>
+        <v>0.25327510917030577</v>
       </c>
       <c r="G67" s="30"/>
-      <c r="H67" s="30"/>
+      <c r="H67" s="30">
+        <v>42790</v>
+      </c>
       <c r="I67" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3945,10 +4013,12 @@
       </c>
       <c r="F68" s="15">
         <f t="shared" si="6"/>
-        <v>0.24686192468619247</v>
+        <v>0.25764192139738001</v>
       </c>
       <c r="G68" s="30"/>
-      <c r="H68" s="30"/>
+      <c r="H68" s="30">
+        <v>42790</v>
+      </c>
       <c r="I68" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3972,10 +4042,12 @@
       </c>
       <c r="F69" s="15">
         <f t="shared" si="6"/>
-        <v>0.24965132496513251</v>
+        <v>0.26055312954876286</v>
       </c>
       <c r="G69" s="30"/>
-      <c r="H69" s="30"/>
+      <c r="H69" s="30">
+        <v>42790</v>
+      </c>
       <c r="I69" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -3999,10 +4071,12 @@
       </c>
       <c r="F70" s="15">
         <f t="shared" si="6"/>
-        <v>0.25244072524407252</v>
+        <v>0.26346433770014571</v>
       </c>
       <c r="G70" s="30"/>
-      <c r="H70" s="30"/>
+      <c r="H70" s="30">
+        <v>42790</v>
+      </c>
       <c r="I70" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -4026,10 +4100,12 @@
       </c>
       <c r="F71" s="15">
         <f t="shared" si="6"/>
-        <v>0.25662482566248257</v>
+        <v>0.26783114992721996</v>
       </c>
       <c r="G71" s="30"/>
-      <c r="H71" s="30"/>
+      <c r="H71" s="30">
+        <v>42790</v>
+      </c>
       <c r="I71" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -4053,10 +4129,12 @@
       </c>
       <c r="F72" s="15">
         <f t="shared" ref="F72:F135" si="14">F71+(C72/$C$197)</f>
-        <v>0.26638772663877269</v>
+        <v>0.27802037845705985</v>
       </c>
       <c r="G72" s="30"/>
-      <c r="H72" s="30"/>
+      <c r="H72" s="30">
+        <v>42790</v>
+      </c>
       <c r="I72" s="9" t="str">
         <f t="shared" ref="I72:I135" si="15">IF(H72="", "", IF(ISBLANK(H73), IF(H72&lt;&gt;H74, SUMIF(H:H,H72,C:C), ""), IF(H72&lt;&gt;H73, SUMIF(H:H,H72,C:C), "")))</f>
         <v/>
@@ -4080,10 +4158,12 @@
       </c>
       <c r="F73" s="15">
         <f t="shared" si="14"/>
-        <v>0.27196652719665276</v>
+        <v>0.28384279475982549</v>
       </c>
       <c r="G73" s="30"/>
-      <c r="H73" s="30"/>
+      <c r="H73" s="30">
+        <v>42790</v>
+      </c>
       <c r="I73" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4107,10 +4187,12 @@
       </c>
       <c r="F74" s="15">
         <f t="shared" si="14"/>
-        <v>0.27894002789400285</v>
+        <v>0.29112081513828253</v>
       </c>
       <c r="G74" s="30"/>
-      <c r="H74" s="30"/>
+      <c r="H74" s="30">
+        <v>42790</v>
+      </c>
       <c r="I74" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4134,10 +4216,12 @@
       </c>
       <c r="F75" s="15">
         <f t="shared" si="14"/>
-        <v>0.31380753138075318</v>
+        <v>0.32751091703056784</v>
       </c>
       <c r="G75" s="30"/>
-      <c r="H75" s="30"/>
+      <c r="H75" s="30">
+        <v>42790</v>
+      </c>
       <c r="I75" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4161,17 +4245,19 @@
       </c>
       <c r="F76" s="15">
         <f t="shared" si="14"/>
-        <v>0.32078103207810327</v>
+        <v>0.33478893740902488</v>
       </c>
       <c r="G76" s="30"/>
-      <c r="H76" s="30"/>
-      <c r="I76" s="9" t="str">
+      <c r="H76" s="30">
+        <v>42790</v>
+      </c>
+      <c r="I76" s="9">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="J76" s="38" t="str">
+        <v>65</v>
+      </c>
+      <c r="J76" s="38">
         <f t="shared" si="16"/>
-        <v/>
+        <v>1.0833333333333333</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="21" thickBot="1">
@@ -4187,7 +4273,7 @@
       <c r="E77" s="27"/>
       <c r="F77" s="29">
         <f t="shared" si="14"/>
-        <v>0.32078103207810327</v>
+        <v>0.33478893740902488</v>
       </c>
       <c r="G77" s="41" t="str">
         <f>IF(COUNTA(G78:G101)=COUNTA(B78:B101), "COMPLETE", "")</f>
@@ -4219,10 +4305,12 @@
       </c>
       <c r="F78" s="15">
         <f t="shared" si="14"/>
-        <v>0.32496513249651332</v>
+        <v>0.33915574963609912</v>
       </c>
       <c r="G78" s="30"/>
-      <c r="H78" s="30"/>
+      <c r="H78" s="30">
+        <v>42791</v>
+      </c>
       <c r="I78" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4246,10 +4334,12 @@
       </c>
       <c r="F79" s="15">
         <f t="shared" si="14"/>
-        <v>0.33054393305439339</v>
+        <v>0.34497816593886477</v>
       </c>
       <c r="G79" s="30"/>
-      <c r="H79" s="30"/>
+      <c r="H79" s="30">
+        <v>42791</v>
+      </c>
       <c r="I79" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4273,10 +4363,12 @@
       </c>
       <c r="F80" s="15">
         <f t="shared" si="14"/>
-        <v>0.3389121338912135</v>
+        <v>0.35371179039301326</v>
       </c>
       <c r="G80" s="30"/>
-      <c r="H80" s="30"/>
+      <c r="H80" s="30">
+        <v>42791</v>
+      </c>
       <c r="I80" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4300,10 +4392,12 @@
       </c>
       <c r="F81" s="15">
         <f t="shared" si="14"/>
-        <v>0.34309623430962355</v>
+        <v>0.3580786026200875</v>
       </c>
       <c r="G81" s="30"/>
-      <c r="H81" s="30"/>
+      <c r="H81" s="30">
+        <v>42791</v>
+      </c>
       <c r="I81" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4327,10 +4421,12 @@
       </c>
       <c r="F82" s="15">
         <f t="shared" si="14"/>
-        <v>0.3472803347280336</v>
+        <v>0.36244541484716175</v>
       </c>
       <c r="G82" s="30"/>
-      <c r="H82" s="30"/>
+      <c r="H82" s="30">
+        <v>42791</v>
+      </c>
       <c r="I82" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4354,10 +4450,12 @@
       </c>
       <c r="F83" s="15">
         <f t="shared" si="14"/>
-        <v>0.35146443514644365</v>
+        <v>0.366812227074236</v>
       </c>
       <c r="G83" s="30"/>
-      <c r="H83" s="30"/>
+      <c r="H83" s="30">
+        <v>42791</v>
+      </c>
       <c r="I83" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4381,10 +4479,12 @@
       </c>
       <c r="F84" s="15">
         <f t="shared" si="14"/>
-        <v>0.35425383542538369</v>
+        <v>0.36972343522561885</v>
       </c>
       <c r="G84" s="30"/>
-      <c r="H84" s="30"/>
+      <c r="H84" s="30">
+        <v>42791</v>
+      </c>
       <c r="I84" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4408,10 +4508,12 @@
       </c>
       <c r="F85" s="15">
         <f t="shared" si="14"/>
-        <v>0.36122733612273378</v>
+        <v>0.37700145560407589</v>
       </c>
       <c r="G85" s="30"/>
-      <c r="H85" s="30"/>
+      <c r="H85" s="30">
+        <v>42791</v>
+      </c>
       <c r="I85" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4435,10 +4537,12 @@
       </c>
       <c r="F86" s="15">
         <f t="shared" si="14"/>
-        <v>0.3709902370990239</v>
+        <v>0.38719068413391577</v>
       </c>
       <c r="G86" s="30"/>
-      <c r="H86" s="30"/>
+      <c r="H86" s="30">
+        <v>42791</v>
+      </c>
       <c r="I86" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4462,10 +4566,12 @@
       </c>
       <c r="F87" s="15">
         <f t="shared" si="14"/>
-        <v>0.37656903765690397</v>
+        <v>0.39301310043668142</v>
       </c>
       <c r="G87" s="30"/>
-      <c r="H87" s="30"/>
+      <c r="H87" s="30">
+        <v>42791</v>
+      </c>
       <c r="I87" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4489,10 +4595,12 @@
       </c>
       <c r="F88" s="15">
         <f t="shared" si="14"/>
-        <v>0.38214783821478404</v>
+        <v>0.39883551673944706</v>
       </c>
       <c r="G88" s="30"/>
-      <c r="H88" s="30"/>
+      <c r="H88" s="30">
+        <v>42791</v>
+      </c>
       <c r="I88" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4516,10 +4624,12 @@
       </c>
       <c r="F89" s="15">
         <f t="shared" si="14"/>
-        <v>0.38354253835425406</v>
+        <v>0.40029112081513846</v>
       </c>
       <c r="G89" s="30"/>
-      <c r="H89" s="30"/>
+      <c r="H89" s="30">
+        <v>42791</v>
+      </c>
       <c r="I89" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4543,10 +4653,12 @@
       </c>
       <c r="F90" s="15">
         <f t="shared" si="14"/>
-        <v>0.38633193863319409</v>
+        <v>0.40320232896652131</v>
       </c>
       <c r="G90" s="30"/>
-      <c r="H90" s="30"/>
+      <c r="H90" s="30">
+        <v>42791</v>
+      </c>
       <c r="I90" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4570,10 +4682,12 @@
       </c>
       <c r="F91" s="15">
         <f t="shared" si="14"/>
-        <v>0.38912133891213413</v>
+        <v>0.40611353711790416</v>
       </c>
       <c r="G91" s="30"/>
-      <c r="H91" s="30"/>
+      <c r="H91" s="30">
+        <v>42791</v>
+      </c>
       <c r="I91" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4597,10 +4711,12 @@
       </c>
       <c r="F92" s="15">
         <f t="shared" si="14"/>
-        <v>0.39330543933054418</v>
+        <v>0.4104803493449784</v>
       </c>
       <c r="G92" s="30"/>
-      <c r="H92" s="30"/>
+      <c r="H92" s="30">
+        <v>42791</v>
+      </c>
       <c r="I92" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4624,17 +4740,19 @@
       </c>
       <c r="F93" s="15">
         <f t="shared" si="14"/>
-        <v>0.40027894002789427</v>
+        <v>0.41775836972343544</v>
       </c>
       <c r="G93" s="30"/>
-      <c r="H93" s="30"/>
-      <c r="I93" s="9" t="str">
+      <c r="H93" s="30">
+        <v>42791</v>
+      </c>
+      <c r="I93" s="9">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="J93" s="38" t="str">
+        <v>57</v>
+      </c>
+      <c r="J93" s="38">
         <f t="shared" si="16"/>
-        <v/>
+        <v>0.95</v>
       </c>
     </row>
     <row r="94" spans="2:10" outlineLevel="1">
@@ -4651,10 +4769,12 @@
       </c>
       <c r="F94" s="15">
         <f t="shared" si="14"/>
-        <v>0.40585774058577434</v>
+        <v>0.42358078602620108</v>
       </c>
       <c r="G94" s="30"/>
-      <c r="H94" s="30"/>
+      <c r="H94" s="30">
+        <v>42792</v>
+      </c>
       <c r="I94" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4678,10 +4798,12 @@
       </c>
       <c r="F95" s="15">
         <f t="shared" si="14"/>
-        <v>0.41143654114365441</v>
+        <v>0.42940320232896673</v>
       </c>
       <c r="G95" s="30"/>
-      <c r="H95" s="30"/>
+      <c r="H95" s="30">
+        <v>42792</v>
+      </c>
       <c r="I95" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4705,10 +4827,12 @@
       </c>
       <c r="F96" s="15">
         <f t="shared" si="14"/>
-        <v>0.41422594142259445</v>
+        <v>0.43231441048034958</v>
       </c>
       <c r="G96" s="30"/>
-      <c r="H96" s="30"/>
+      <c r="H96" s="30">
+        <v>42792</v>
+      </c>
       <c r="I96" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4732,10 +4856,12 @@
       </c>
       <c r="F97" s="15">
         <f t="shared" si="14"/>
-        <v>0.41701534170153448</v>
+        <v>0.43522561863173242</v>
       </c>
       <c r="G97" s="30"/>
-      <c r="H97" s="30"/>
+      <c r="H97" s="30">
+        <v>42792</v>
+      </c>
       <c r="I97" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4759,10 +4885,12 @@
       </c>
       <c r="F98" s="15">
         <f t="shared" si="14"/>
-        <v>0.41980474198047452</v>
+        <v>0.43813682678311527</v>
       </c>
       <c r="G98" s="30"/>
-      <c r="H98" s="30"/>
+      <c r="H98" s="30">
+        <v>42792</v>
+      </c>
       <c r="I98" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4786,10 +4914,12 @@
       </c>
       <c r="F99" s="15">
         <f t="shared" si="14"/>
-        <v>0.42119944211994453</v>
+        <v>0.43959243085880667</v>
       </c>
       <c r="G99" s="30"/>
-      <c r="H99" s="30"/>
+      <c r="H99" s="30">
+        <v>42792</v>
+      </c>
       <c r="I99" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4813,10 +4943,12 @@
       </c>
       <c r="F100" s="15">
         <f t="shared" si="14"/>
-        <v>0.42398884239888457</v>
+        <v>0.44250363901018952</v>
       </c>
       <c r="G100" s="30"/>
-      <c r="H100" s="30"/>
+      <c r="H100" s="30">
+        <v>42792</v>
+      </c>
       <c r="I100" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4840,10 +4972,12 @@
       </c>
       <c r="F101" s="15">
         <f t="shared" si="14"/>
-        <v>0.43096234309623466</v>
+        <v>0.44978165938864656</v>
       </c>
       <c r="G101" s="30"/>
-      <c r="H101" s="30"/>
+      <c r="H101" s="30">
+        <v>42792</v>
+      </c>
       <c r="I101" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4866,7 +5000,7 @@
       <c r="E102" s="27"/>
       <c r="F102" s="29">
         <f t="shared" si="14"/>
-        <v>0.43096234309623466</v>
+        <v>0.44978165938864656</v>
       </c>
       <c r="G102" s="41" t="str">
         <f>IF(COUNTA(G103:G116)=COUNTA(B103:B116), "COMPLETE", "")</f>
@@ -4898,10 +5032,12 @@
       </c>
       <c r="F103" s="15">
         <f t="shared" si="14"/>
-        <v>0.43654114365411473</v>
+        <v>0.4556040756914122</v>
       </c>
       <c r="G103" s="30"/>
-      <c r="H103" s="30"/>
+      <c r="H103" s="30">
+        <v>42792</v>
+      </c>
       <c r="I103" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4925,10 +5061,12 @@
       </c>
       <c r="F104" s="15">
         <f t="shared" si="14"/>
-        <v>0.43933054393305476</v>
+        <v>0.45851528384279505</v>
       </c>
       <c r="G104" s="30"/>
-      <c r="H104" s="30"/>
+      <c r="H104" s="30">
+        <v>42792</v>
+      </c>
       <c r="I104" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4952,10 +5090,12 @@
       </c>
       <c r="F105" s="15">
         <f t="shared" si="14"/>
-        <v>0.44351464435146482</v>
+        <v>0.4628820960698693</v>
       </c>
       <c r="G105" s="30"/>
-      <c r="H105" s="30"/>
+      <c r="H105" s="30">
+        <v>42792</v>
+      </c>
       <c r="I105" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4979,10 +5119,12 @@
       </c>
       <c r="F106" s="15">
         <f t="shared" si="14"/>
-        <v>0.44490934449093483</v>
+        <v>0.46433770014556069</v>
       </c>
       <c r="G106" s="30"/>
-      <c r="H106" s="30"/>
+      <c r="H106" s="30">
+        <v>42792</v>
+      </c>
       <c r="I106" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5006,10 +5148,12 @@
       </c>
       <c r="F107" s="15">
         <f t="shared" si="14"/>
-        <v>0.44909344490934489</v>
+        <v>0.46870451237263494</v>
       </c>
       <c r="G107" s="30"/>
-      <c r="H107" s="30"/>
+      <c r="H107" s="30">
+        <v>42792</v>
+      </c>
       <c r="I107" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5033,10 +5177,12 @@
       </c>
       <c r="F108" s="15">
         <f t="shared" si="14"/>
-        <v>0.45188284518828492</v>
+        <v>0.47161572052401779</v>
       </c>
       <c r="G108" s="30"/>
-      <c r="H108" s="30"/>
+      <c r="H108" s="30">
+        <v>42792</v>
+      </c>
       <c r="I108" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5060,10 +5206,12 @@
       </c>
       <c r="F109" s="15">
         <f t="shared" si="14"/>
-        <v>0.45606694560669497</v>
+        <v>0.47598253275109204</v>
       </c>
       <c r="G109" s="30"/>
-      <c r="H109" s="30"/>
+      <c r="H109" s="30">
+        <v>42792</v>
+      </c>
       <c r="I109" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5087,10 +5235,12 @@
       </c>
       <c r="F110" s="15">
         <f t="shared" si="14"/>
-        <v>0.45885634588563501</v>
+        <v>0.47889374090247488</v>
       </c>
       <c r="G110" s="30"/>
-      <c r="H110" s="30"/>
+      <c r="H110" s="30">
+        <v>42792</v>
+      </c>
       <c r="I110" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5114,10 +5264,12 @@
       </c>
       <c r="F111" s="15">
         <f t="shared" si="14"/>
-        <v>0.46025104602510503</v>
+        <v>0.48034934497816628</v>
       </c>
       <c r="G111" s="30"/>
-      <c r="H111" s="30"/>
+      <c r="H111" s="30">
+        <v>42792</v>
+      </c>
       <c r="I111" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5141,10 +5293,12 @@
       </c>
       <c r="F112" s="15">
         <f t="shared" si="14"/>
-        <v>0.46722454672245511</v>
+        <v>0.48762736535662332</v>
       </c>
       <c r="G112" s="30"/>
-      <c r="H112" s="30"/>
+      <c r="H112" s="30">
+        <v>42792</v>
+      </c>
       <c r="I112" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5168,10 +5322,12 @@
       </c>
       <c r="F113" s="15">
         <f t="shared" si="14"/>
-        <v>0.47140864714086517</v>
+        <v>0.49199417758369757</v>
       </c>
       <c r="G113" s="30"/>
-      <c r="H113" s="30"/>
+      <c r="H113" s="30">
+        <v>42792</v>
+      </c>
       <c r="I113" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5195,10 +5351,12 @@
       </c>
       <c r="F114" s="15">
         <f t="shared" si="14"/>
-        <v>0.47559274755927522</v>
+        <v>0.49636098981077181</v>
       </c>
       <c r="G114" s="30"/>
-      <c r="H114" s="30"/>
+      <c r="H114" s="30">
+        <v>42792</v>
+      </c>
       <c r="I114" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5222,10 +5380,12 @@
       </c>
       <c r="F115" s="15">
         <f t="shared" si="14"/>
-        <v>0.47977684797768527</v>
+        <v>0.50072780203784606</v>
       </c>
       <c r="G115" s="30"/>
-      <c r="H115" s="30"/>
+      <c r="H115" s="30">
+        <v>42792</v>
+      </c>
       <c r="I115" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5249,17 +5409,19 @@
       </c>
       <c r="F116" s="15">
         <f t="shared" si="14"/>
-        <v>0.48675034867503536</v>
+        <v>0.5080058224163031</v>
       </c>
       <c r="G116" s="30"/>
-      <c r="H116" s="30"/>
-      <c r="I116" s="9" t="str">
+      <c r="H116" s="30">
+        <v>42792</v>
+      </c>
+      <c r="I116" s="9">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="J116" s="38" t="str">
+        <v>62</v>
+      </c>
+      <c r="J116" s="38">
         <f t="shared" si="16"/>
-        <v/>
+        <v>1.0333333333333334</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="21" thickBot="1">
@@ -5275,7 +5437,7 @@
       <c r="E117" s="27"/>
       <c r="F117" s="29">
         <f t="shared" si="14"/>
-        <v>0.48675034867503536</v>
+        <v>0.5080058224163031</v>
       </c>
       <c r="G117" s="41" t="str">
         <f>IF(COUNTA(G118:G134)=COUNTA(B118:B134), "COMPLETE", "")</f>
@@ -5307,10 +5469,12 @@
       </c>
       <c r="F118" s="15">
         <f t="shared" si="14"/>
-        <v>0.49372384937238545</v>
+        <v>0.51528384279476014</v>
       </c>
       <c r="G118" s="30"/>
-      <c r="H118" s="30"/>
+      <c r="H118" s="30">
+        <v>42793</v>
+      </c>
       <c r="I118" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5334,10 +5498,12 @@
       </c>
       <c r="F119" s="15">
         <f t="shared" si="14"/>
-        <v>0.49651324965132548</v>
+        <v>0.51819505094614293</v>
       </c>
       <c r="G119" s="30"/>
-      <c r="H119" s="30"/>
+      <c r="H119" s="30">
+        <v>42793</v>
+      </c>
       <c r="I119" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5361,10 +5527,12 @@
       </c>
       <c r="F120" s="15">
         <f t="shared" si="14"/>
-        <v>0.50069735006973548</v>
+        <v>0.52256186317321718</v>
       </c>
       <c r="G120" s="30"/>
-      <c r="H120" s="30"/>
+      <c r="H120" s="30">
+        <v>42793</v>
+      </c>
       <c r="I120" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5388,10 +5556,12 @@
       </c>
       <c r="F121" s="15">
         <f t="shared" si="14"/>
-        <v>0.50348675034867552</v>
+        <v>0.52547307132459997</v>
       </c>
       <c r="G121" s="30"/>
-      <c r="H121" s="30"/>
+      <c r="H121" s="30">
+        <v>42793</v>
+      </c>
       <c r="I121" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5415,10 +5585,12 @@
       </c>
       <c r="F122" s="15">
         <f t="shared" si="14"/>
-        <v>0.50906555090655559</v>
+        <v>0.53129548762736567</v>
       </c>
       <c r="G122" s="30"/>
-      <c r="H122" s="30"/>
+      <c r="H122" s="30">
+        <v>42793</v>
+      </c>
       <c r="I122" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5442,10 +5614,12 @@
       </c>
       <c r="F123" s="15">
         <f t="shared" si="14"/>
-        <v>0.51185495118549562</v>
+        <v>0.53420669577874846</v>
       </c>
       <c r="G123" s="30"/>
-      <c r="H123" s="30"/>
+      <c r="H123" s="30">
+        <v>42793</v>
+      </c>
       <c r="I123" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5469,10 +5643,12 @@
       </c>
       <c r="F124" s="15">
         <f t="shared" si="14"/>
-        <v>0.51324965132496558</v>
+        <v>0.53566229985443992</v>
       </c>
       <c r="G124" s="30"/>
-      <c r="H124" s="30"/>
+      <c r="H124" s="30">
+        <v>42793</v>
+      </c>
       <c r="I124" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5496,10 +5672,12 @@
       </c>
       <c r="F125" s="15">
         <f t="shared" si="14"/>
-        <v>0.51743375174337558</v>
+        <v>0.54002911208151416</v>
       </c>
       <c r="G125" s="30"/>
-      <c r="H125" s="30"/>
+      <c r="H125" s="30">
+        <v>42793</v>
+      </c>
       <c r="I125" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5523,10 +5701,12 @@
       </c>
       <c r="F126" s="15">
         <f t="shared" si="14"/>
-        <v>0.52022315202231562</v>
+        <v>0.54294032023289696</v>
       </c>
       <c r="G126" s="30"/>
-      <c r="H126" s="30"/>
+      <c r="H126" s="30">
+        <v>42793</v>
+      </c>
       <c r="I126" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5550,10 +5730,12 @@
       </c>
       <c r="F127" s="15">
         <f t="shared" si="14"/>
-        <v>0.52301255230125565</v>
+        <v>0.54585152838427975</v>
       </c>
       <c r="G127" s="30"/>
-      <c r="H127" s="30"/>
+      <c r="H127" s="30">
+        <v>42793</v>
+      </c>
       <c r="I127" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5577,10 +5759,12 @@
       </c>
       <c r="F128" s="15">
         <f t="shared" si="14"/>
-        <v>0.52998605299860568</v>
+        <v>0.55312954876273679</v>
       </c>
       <c r="G128" s="30"/>
-      <c r="H128" s="30"/>
+      <c r="H128" s="30">
+        <v>42793</v>
+      </c>
       <c r="I128" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5604,10 +5788,12 @@
       </c>
       <c r="F129" s="15">
         <f t="shared" si="14"/>
-        <v>0.53417015341701568</v>
+        <v>0.55749636098981104</v>
       </c>
       <c r="G129" s="30"/>
-      <c r="H129" s="30"/>
+      <c r="H129" s="30">
+        <v>42793</v>
+      </c>
       <c r="I129" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5631,10 +5817,12 @@
       </c>
       <c r="F130" s="15">
         <f t="shared" si="14"/>
-        <v>0.53556485355648564</v>
+        <v>0.55895196506550249</v>
       </c>
       <c r="G130" s="30"/>
-      <c r="H130" s="30"/>
+      <c r="H130" s="30">
+        <v>42793</v>
+      </c>
       <c r="I130" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5658,10 +5846,12 @@
       </c>
       <c r="F131" s="15">
         <f t="shared" si="14"/>
-        <v>0.5369595536959556</v>
+        <v>0.56040756914119394</v>
       </c>
       <c r="G131" s="30"/>
-      <c r="H131" s="30"/>
+      <c r="H131" s="30">
+        <v>42793</v>
+      </c>
       <c r="I131" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5685,10 +5875,12 @@
       </c>
       <c r="F132" s="15">
         <f t="shared" si="14"/>
-        <v>0.53835425383542557</v>
+        <v>0.56186317321688539</v>
       </c>
       <c r="G132" s="30"/>
-      <c r="H132" s="30"/>
+      <c r="H132" s="30">
+        <v>42793</v>
+      </c>
       <c r="I132" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5712,10 +5904,12 @@
       </c>
       <c r="F133" s="15">
         <f t="shared" si="14"/>
-        <v>0.53974895397489553</v>
+        <v>0.56331877729257684</v>
       </c>
       <c r="G133" s="30"/>
-      <c r="H133" s="30"/>
+      <c r="H133" s="30">
+        <v>42793</v>
+      </c>
       <c r="I133" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5739,17 +5933,19 @@
       </c>
       <c r="F134" s="15">
         <f t="shared" si="14"/>
-        <v>0.54253835425383556</v>
+        <v>0.56622998544395964</v>
       </c>
       <c r="G134" s="30"/>
-      <c r="H134" s="30"/>
-      <c r="I134" s="9" t="str">
+      <c r="H134" s="30">
+        <v>42793</v>
+      </c>
+      <c r="I134" s="9">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="J134" s="38" t="str">
+        <v>40</v>
+      </c>
+      <c r="J134" s="38">
         <f t="shared" si="16"/>
-        <v/>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="135" spans="1:10" ht="21" thickBot="1">
@@ -5760,12 +5956,12 @@
       <c r="C135" s="26"/>
       <c r="D135" s="20">
         <f>SUM(C135:C174)</f>
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="E135" s="27"/>
       <c r="F135" s="29">
         <f t="shared" si="14"/>
-        <v>0.54253835425383556</v>
+        <v>0.56622998544395964</v>
       </c>
       <c r="G135" s="41" t="str">
         <f>IF(COUNTA(G136:G173)=COUNTA(B136:B173), "COMPLETE", "")</f>
@@ -5789,18 +5985,20 @@
       </c>
       <c r="D136" s="21">
         <f>D135/60</f>
-        <v>3.4</v>
+        <v>2.9</v>
       </c>
       <c r="E136" s="15">
         <f>E135+(C136/$D$135)</f>
-        <v>1.9607843137254902E-2</v>
+        <v>2.2988505747126436E-2</v>
       </c>
       <c r="F136" s="15">
         <f t="shared" ref="F136:F195" si="21">F135+(C136/$C$197)</f>
-        <v>0.54811715481171563</v>
+        <v>0.57205240174672534</v>
       </c>
       <c r="G136" s="30"/>
-      <c r="H136" s="30"/>
+      <c r="H136" s="30">
+        <v>42794</v>
+      </c>
       <c r="I136" s="9" t="str">
         <f t="shared" ref="I136:I195" si="22">IF(H136="", "", IF(ISBLANK(H137), IF(H136&lt;&gt;H138, SUMIF(H:H,H136,C:C), ""), IF(H136&lt;&gt;H137, SUMIF(H:H,H136,C:C), "")))</f>
         <v/>
@@ -5820,14 +6018,16 @@
       <c r="D137" s="19"/>
       <c r="E137" s="15">
         <f t="shared" ref="E137:E173" si="24">E136+(C137/$D$135)</f>
-        <v>3.9215686274509803E-2</v>
+        <v>4.5977011494252873E-2</v>
       </c>
       <c r="F137" s="15">
         <f t="shared" si="21"/>
-        <v>0.5536959553695957</v>
+        <v>0.57787481804949103</v>
       </c>
       <c r="G137" s="30"/>
-      <c r="H137" s="30"/>
+      <c r="H137" s="30">
+        <v>42794</v>
+      </c>
       <c r="I137" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5847,14 +6047,16 @@
       <c r="D138" s="19"/>
       <c r="E138" s="15">
         <f t="shared" si="24"/>
-        <v>5.8823529411764705E-2</v>
+        <v>6.8965517241379309E-2</v>
       </c>
       <c r="F138" s="15">
         <f t="shared" si="21"/>
-        <v>0.55927475592747578</v>
+        <v>0.58369723435225673</v>
       </c>
       <c r="G138" s="30"/>
-      <c r="H138" s="30"/>
+      <c r="H138" s="30">
+        <v>42794</v>
+      </c>
       <c r="I138" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5874,14 +6076,16 @@
       <c r="D139" s="19"/>
       <c r="E139" s="15">
         <f t="shared" si="24"/>
-        <v>7.8431372549019607E-2</v>
+        <v>9.1954022988505746E-2</v>
       </c>
       <c r="F139" s="15">
         <f t="shared" si="21"/>
-        <v>0.56485355648535585</v>
+        <v>0.58951965065502243</v>
       </c>
       <c r="G139" s="30"/>
-      <c r="H139" s="30"/>
+      <c r="H139" s="30">
+        <v>42794</v>
+      </c>
       <c r="I139" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5901,14 +6105,16 @@
       <c r="D140" s="19"/>
       <c r="E140" s="15">
         <f t="shared" si="24"/>
-        <v>9.3137254901960786E-2</v>
+        <v>0.10919540229885058</v>
       </c>
       <c r="F140" s="15">
         <f t="shared" si="21"/>
-        <v>0.56903765690376584</v>
+        <v>0.59388646288209668</v>
       </c>
       <c r="G140" s="30"/>
-      <c r="H140" s="30"/>
+      <c r="H140" s="30">
+        <v>42794</v>
+      </c>
       <c r="I140" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5928,14 +6134,16 @@
       <c r="D141" s="19"/>
       <c r="E141" s="15">
         <f t="shared" si="24"/>
-        <v>0.10294117647058823</v>
+        <v>0.1206896551724138</v>
       </c>
       <c r="F141" s="15">
         <f t="shared" si="21"/>
-        <v>0.57182705718270588</v>
+        <v>0.59679767103347947</v>
       </c>
       <c r="G141" s="30"/>
-      <c r="H141" s="30"/>
+      <c r="H141" s="30">
+        <v>42794</v>
+      </c>
       <c r="I141" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5955,14 +6163,16 @@
       <c r="D142" s="19"/>
       <c r="E142" s="15">
         <f t="shared" si="24"/>
-        <v>0.12254901960784313</v>
+        <v>0.14367816091954022</v>
       </c>
       <c r="F142" s="15">
         <f t="shared" si="21"/>
-        <v>0.57740585774058595</v>
+        <v>0.60262008733624517</v>
       </c>
       <c r="G142" s="30"/>
-      <c r="H142" s="30"/>
+      <c r="H142" s="30">
+        <v>42794</v>
+      </c>
       <c r="I142" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -5982,14 +6192,16 @@
       <c r="D143" s="19"/>
       <c r="E143" s="15">
         <f t="shared" si="24"/>
-        <v>0.15686274509803921</v>
+        <v>0.18390804597701149</v>
       </c>
       <c r="F143" s="15">
         <f t="shared" si="21"/>
-        <v>0.58716875871687602</v>
+        <v>0.612809315866085</v>
       </c>
       <c r="G143" s="30"/>
-      <c r="H143" s="30"/>
+      <c r="H143" s="30">
+        <v>42794</v>
+      </c>
       <c r="I143" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6009,14 +6221,16 @@
       <c r="D144" s="19"/>
       <c r="E144" s="15">
         <f t="shared" si="24"/>
-        <v>0.16176470588235295</v>
+        <v>0.18965517241379309</v>
       </c>
       <c r="F144" s="15">
         <f t="shared" si="21"/>
-        <v>0.58856345885634598</v>
+        <v>0.61426491994177645</v>
       </c>
       <c r="G144" s="30"/>
-      <c r="H144" s="30"/>
+      <c r="H144" s="30">
+        <v>42794</v>
+      </c>
       <c r="I144" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6036,14 +6250,16 @@
       <c r="D145" s="19"/>
       <c r="E145" s="15">
         <f t="shared" si="24"/>
-        <v>0.17647058823529413</v>
+        <v>0.20689655172413793</v>
       </c>
       <c r="F145" s="15">
         <f t="shared" si="21"/>
-        <v>0.59274755927475598</v>
+        <v>0.6186317321688507</v>
       </c>
       <c r="G145" s="30"/>
-      <c r="H145" s="30"/>
+      <c r="H145" s="30">
+        <v>42794</v>
+      </c>
       <c r="I145" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6063,14 +6279,16 @@
       <c r="D146" s="19"/>
       <c r="E146" s="15">
         <f t="shared" si="24"/>
-        <v>0.18627450980392157</v>
+        <v>0.21839080459770116</v>
       </c>
       <c r="F146" s="15">
         <f t="shared" si="21"/>
-        <v>0.59553695955369601</v>
+        <v>0.62154294032023349</v>
       </c>
       <c r="G146" s="30"/>
-      <c r="H146" s="30"/>
+      <c r="H146" s="30">
+        <v>42794</v>
+      </c>
       <c r="I146" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6090,14 +6308,16 @@
       <c r="D147" s="19"/>
       <c r="E147" s="15">
         <f t="shared" si="24"/>
-        <v>0.19607843137254902</v>
+        <v>0.22988505747126436</v>
       </c>
       <c r="F147" s="15">
         <f t="shared" si="21"/>
-        <v>0.59832635983263605</v>
+        <v>0.62445414847161629</v>
       </c>
       <c r="G147" s="30"/>
-      <c r="H147" s="30"/>
+      <c r="H147" s="30">
+        <v>42794</v>
+      </c>
       <c r="I147" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6117,14 +6337,16 @@
       <c r="D148" s="19"/>
       <c r="E148" s="15">
         <f t="shared" si="24"/>
-        <v>0.2107843137254902</v>
+        <v>0.2471264367816092</v>
       </c>
       <c r="F148" s="15">
         <f t="shared" si="21"/>
-        <v>0.60251046025104604</v>
+        <v>0.62882096069869053</v>
       </c>
       <c r="G148" s="30"/>
-      <c r="H148" s="30"/>
+      <c r="H148" s="30">
+        <v>42794</v>
+      </c>
       <c r="I148" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6144,14 +6366,16 @@
       <c r="D149" s="19"/>
       <c r="E149" s="15">
         <f t="shared" si="24"/>
-        <v>0.22549019607843138</v>
+        <v>0.26436781609195403</v>
       </c>
       <c r="F149" s="15">
         <f t="shared" si="21"/>
-        <v>0.60669456066945604</v>
+        <v>0.63318777292576478</v>
       </c>
       <c r="G149" s="30"/>
-      <c r="H149" s="30"/>
+      <c r="H149" s="30">
+        <v>42794</v>
+      </c>
       <c r="I149" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6171,14 +6395,16 @@
       <c r="D150" s="19"/>
       <c r="E150" s="15">
         <f t="shared" si="24"/>
-        <v>0.25</v>
+        <v>0.2931034482758621</v>
       </c>
       <c r="F150" s="15">
         <f t="shared" si="21"/>
-        <v>0.61366806136680607</v>
+        <v>0.64046579330422182</v>
       </c>
       <c r="G150" s="30"/>
-      <c r="H150" s="30"/>
+      <c r="H150" s="30">
+        <v>42794</v>
+      </c>
       <c r="I150" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6190,22 +6416,24 @@
     </row>
     <row r="151" spans="2:10" outlineLevel="1">
       <c r="B151" s="18" t="s">
-        <v>178</v>
+        <v>249</v>
       </c>
       <c r="C151" s="13">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D151" s="19"/>
       <c r="E151" s="15">
         <f t="shared" si="24"/>
-        <v>0.31862745098039214</v>
+        <v>0.31609195402298851</v>
       </c>
       <c r="F151" s="15">
         <f t="shared" si="21"/>
-        <v>0.63319386331938632</v>
+        <v>0.64628820960698752</v>
       </c>
       <c r="G151" s="30"/>
-      <c r="H151" s="30"/>
+      <c r="H151" s="30">
+        <v>42794</v>
+      </c>
       <c r="I151" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6217,29 +6445,31 @@
     </row>
     <row r="152" spans="2:10" outlineLevel="1">
       <c r="B152" s="18" t="s">
-        <v>179</v>
+        <v>248</v>
       </c>
       <c r="C152" s="13">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D152" s="19"/>
       <c r="E152" s="15">
         <f t="shared" si="24"/>
-        <v>0.46568627450980393</v>
+        <v>0.37356321839080459</v>
       </c>
       <c r="F152" s="15">
         <f t="shared" si="21"/>
-        <v>0.67503486750348674</v>
+        <v>0.6608442503639016</v>
       </c>
       <c r="G152" s="30"/>
-      <c r="H152" s="30"/>
-      <c r="I152" s="9" t="str">
+      <c r="H152" s="30">
+        <v>42794</v>
+      </c>
+      <c r="I152" s="9">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="J152" s="38" t="str">
+        <v>65</v>
+      </c>
+      <c r="J152" s="38">
         <f t="shared" si="23"/>
-        <v/>
+        <v>1.0833333333333333</v>
       </c>
     </row>
     <row r="153" spans="2:10" outlineLevel="1">
@@ -6252,14 +6482,16 @@
       <c r="D153" s="19"/>
       <c r="E153" s="15">
         <f t="shared" si="24"/>
-        <v>0.49019607843137258</v>
+        <v>0.40229885057471265</v>
       </c>
       <c r="F153" s="15">
         <f t="shared" si="21"/>
-        <v>0.68200836820083677</v>
+        <v>0.66812227074235864</v>
       </c>
       <c r="G153" s="30"/>
-      <c r="H153" s="30"/>
+      <c r="H153" s="30">
+        <v>42795</v>
+      </c>
       <c r="I153" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6279,14 +6511,16 @@
       <c r="D154" s="19"/>
       <c r="E154" s="15">
         <f t="shared" si="24"/>
-        <v>0.51960784313725494</v>
+        <v>0.43678160919540232</v>
       </c>
       <c r="F154" s="15">
         <f t="shared" si="21"/>
-        <v>0.69037656903765687</v>
+        <v>0.67685589519650713</v>
       </c>
       <c r="G154" s="30"/>
-      <c r="H154" s="30"/>
+      <c r="H154" s="30">
+        <v>42795</v>
+      </c>
       <c r="I154" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6306,14 +6540,16 @@
       <c r="D155" s="19"/>
       <c r="E155" s="15">
         <f t="shared" si="24"/>
-        <v>0.53921568627450989</v>
+        <v>0.45977011494252873</v>
       </c>
       <c r="F155" s="15">
         <f t="shared" si="21"/>
-        <v>0.69595536959553694</v>
+        <v>0.68267831149927283</v>
       </c>
       <c r="G155" s="30"/>
-      <c r="H155" s="30"/>
+      <c r="H155" s="30">
+        <v>42795</v>
+      </c>
       <c r="I155" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6333,14 +6569,16 @@
       <c r="D156" s="19"/>
       <c r="E156" s="15">
         <f t="shared" si="24"/>
-        <v>0.55882352941176483</v>
+        <v>0.48275862068965514</v>
       </c>
       <c r="F156" s="15">
         <f t="shared" si="21"/>
-        <v>0.70153417015341701</v>
+        <v>0.68850072780203853</v>
       </c>
       <c r="G156" s="30"/>
-      <c r="H156" s="30"/>
+      <c r="H156" s="30">
+        <v>42795</v>
+      </c>
       <c r="I156" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6360,14 +6598,16 @@
       <c r="D157" s="19"/>
       <c r="E157" s="15">
         <f t="shared" si="24"/>
-        <v>0.57843137254901977</v>
+        <v>0.50574712643678155</v>
       </c>
       <c r="F157" s="15">
         <f t="shared" si="21"/>
-        <v>0.70711297071129708</v>
+        <v>0.69432314410480422</v>
       </c>
       <c r="G157" s="30"/>
-      <c r="H157" s="30"/>
+      <c r="H157" s="30">
+        <v>42795</v>
+      </c>
       <c r="I157" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6387,14 +6627,16 @@
       <c r="D158" s="19"/>
       <c r="E158" s="15">
         <f t="shared" si="24"/>
-        <v>0.59803921568627472</v>
+        <v>0.52873563218390796</v>
       </c>
       <c r="F158" s="15">
         <f t="shared" si="21"/>
-        <v>0.71269177126917715</v>
+        <v>0.70014556040756992</v>
       </c>
       <c r="G158" s="30"/>
-      <c r="H158" s="30"/>
+      <c r="H158" s="30">
+        <v>42795</v>
+      </c>
       <c r="I158" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6414,14 +6656,16 @@
       <c r="D159" s="19"/>
       <c r="E159" s="15">
         <f t="shared" si="24"/>
-        <v>0.62254901960784337</v>
+        <v>0.55747126436781602</v>
       </c>
       <c r="F159" s="15">
         <f t="shared" si="21"/>
-        <v>0.71966527196652719</v>
+        <v>0.70742358078602696</v>
       </c>
       <c r="G159" s="30"/>
-      <c r="H159" s="30"/>
+      <c r="H159" s="30">
+        <v>42795</v>
+      </c>
       <c r="I159" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6441,14 +6685,16 @@
       <c r="D160" s="19"/>
       <c r="E160" s="15">
         <f t="shared" si="24"/>
-        <v>0.63725490196078449</v>
+        <v>0.57471264367816088</v>
       </c>
       <c r="F160" s="15">
         <f t="shared" si="21"/>
-        <v>0.72384937238493718</v>
+        <v>0.71179039301310121</v>
       </c>
       <c r="G160" s="30"/>
-      <c r="H160" s="30"/>
+      <c r="H160" s="30">
+        <v>42795</v>
+      </c>
       <c r="I160" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6468,14 +6714,16 @@
       <c r="D161" s="19"/>
       <c r="E161" s="15">
         <f t="shared" si="24"/>
-        <v>0.6862745098039218</v>
+        <v>0.63218390804597702</v>
       </c>
       <c r="F161" s="15">
         <f t="shared" si="21"/>
-        <v>0.73779637377963736</v>
+        <v>0.72634643377001529</v>
       </c>
       <c r="G161" s="30"/>
-      <c r="H161" s="30"/>
+      <c r="H161" s="30">
+        <v>42795</v>
+      </c>
       <c r="I161" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6495,14 +6743,16 @@
       <c r="D162" s="19"/>
       <c r="E162" s="15">
         <f t="shared" si="24"/>
-        <v>0.71568627450980415</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="F162" s="15">
         <f t="shared" si="21"/>
-        <v>0.74616457461645747</v>
+        <v>0.73508005822416378</v>
       </c>
       <c r="G162" s="30"/>
-      <c r="H162" s="30"/>
+      <c r="H162" s="30">
+        <v>42795</v>
+      </c>
       <c r="I162" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6522,21 +6772,23 @@
       <c r="D163" s="19"/>
       <c r="E163" s="15">
         <f t="shared" si="24"/>
-        <v>0.75000000000000022</v>
+        <v>0.7068965517241379</v>
       </c>
       <c r="F163" s="15">
         <f t="shared" si="21"/>
-        <v>0.75592747559274753</v>
+        <v>0.74526928675400361</v>
       </c>
       <c r="G163" s="30"/>
-      <c r="H163" s="30"/>
-      <c r="I163" s="9" t="str">
+      <c r="H163" s="30">
+        <v>42795</v>
+      </c>
+      <c r="I163" s="9">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="J163" s="38" t="str">
+        <v>58</v>
+      </c>
+      <c r="J163" s="38">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0.96666666666666667</v>
       </c>
     </row>
     <row r="164" spans="1:10" outlineLevel="1">
@@ -6549,14 +6801,16 @@
       <c r="D164" s="19"/>
       <c r="E164" s="15">
         <f t="shared" si="24"/>
-        <v>0.78921568627451</v>
+        <v>0.75287356321839072</v>
       </c>
       <c r="F164" s="15">
         <f t="shared" si="21"/>
-        <v>0.76708507670850767</v>
+        <v>0.7569141193595349</v>
       </c>
       <c r="G164" s="30"/>
-      <c r="H164" s="30"/>
+      <c r="H164" s="30">
+        <v>42796</v>
+      </c>
       <c r="I164" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6576,14 +6830,16 @@
       <c r="D165" s="19"/>
       <c r="E165" s="15">
         <f t="shared" si="24"/>
-        <v>0.80882352941176494</v>
+        <v>0.77586206896551713</v>
       </c>
       <c r="F165" s="15">
         <f t="shared" si="21"/>
-        <v>0.77266387726638774</v>
+        <v>0.7627365356623006</v>
       </c>
       <c r="G165" s="30"/>
-      <c r="H165" s="30"/>
+      <c r="H165" s="30">
+        <v>42796</v>
+      </c>
       <c r="I165" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6603,14 +6859,16 @@
       <c r="D166" s="19"/>
       <c r="E166" s="15">
         <f t="shared" si="24"/>
-        <v>0.8382352941176473</v>
+        <v>0.81034482758620674</v>
       </c>
       <c r="F166" s="15">
         <f t="shared" si="21"/>
-        <v>0.78103207810320785</v>
+        <v>0.77147016011644909</v>
       </c>
       <c r="G166" s="30"/>
-      <c r="H166" s="30"/>
+      <c r="H166" s="30">
+        <v>42796</v>
+      </c>
       <c r="I166" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6630,14 +6888,16 @@
       <c r="D167" s="19"/>
       <c r="E167" s="15">
         <f t="shared" si="24"/>
-        <v>0.85784313725490224</v>
+        <v>0.83333333333333315</v>
       </c>
       <c r="F167" s="15">
         <f t="shared" si="21"/>
-        <v>0.78661087866108792</v>
+        <v>0.77729257641921479</v>
       </c>
       <c r="G167" s="30"/>
-      <c r="H167" s="30"/>
+      <c r="H167" s="30">
+        <v>42796</v>
+      </c>
       <c r="I167" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6657,14 +6917,16 @@
       <c r="D168" s="19"/>
       <c r="E168" s="15">
         <f t="shared" si="24"/>
-        <v>0.90686274509803955</v>
+        <v>0.89080459770114928</v>
       </c>
       <c r="F168" s="15">
         <f t="shared" si="21"/>
-        <v>0.8005578800557881</v>
+        <v>0.79184861717612887</v>
       </c>
       <c r="G168" s="30"/>
-      <c r="H168" s="30"/>
+      <c r="H168" s="30">
+        <v>42796</v>
+      </c>
       <c r="I168" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6684,14 +6946,16 @@
       <c r="D169" s="19"/>
       <c r="E169" s="15">
         <f t="shared" si="24"/>
-        <v>0.92647058823529449</v>
+        <v>0.91379310344827569</v>
       </c>
       <c r="F169" s="15">
         <f t="shared" si="21"/>
-        <v>0.80613668061366817</v>
+        <v>0.79767103347889456</v>
       </c>
       <c r="G169" s="30"/>
-      <c r="H169" s="30"/>
+      <c r="H169" s="30">
+        <v>42796</v>
+      </c>
       <c r="I169" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6711,14 +6975,16 @@
       <c r="D170" s="19"/>
       <c r="E170" s="15">
         <f t="shared" si="24"/>
-        <v>0.94607843137254943</v>
+        <v>0.9367816091954021</v>
       </c>
       <c r="F170" s="15">
         <f t="shared" si="21"/>
-        <v>0.81171548117154824</v>
+        <v>0.80349344978166026</v>
       </c>
       <c r="G170" s="30"/>
-      <c r="H170" s="30"/>
+      <c r="H170" s="30">
+        <v>42796</v>
+      </c>
       <c r="I170" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6738,14 +7004,16 @@
       <c r="D171" s="19"/>
       <c r="E171" s="15">
         <f t="shared" si="24"/>
-        <v>0.97549019607843179</v>
+        <v>0.97126436781609171</v>
       </c>
       <c r="F171" s="15">
         <f t="shared" si="21"/>
-        <v>0.82008368200836834</v>
+        <v>0.81222707423580875</v>
       </c>
       <c r="G171" s="30"/>
-      <c r="H171" s="30"/>
+      <c r="H171" s="30">
+        <v>42796</v>
+      </c>
       <c r="I171" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6765,14 +7033,16 @@
       <c r="D172" s="19"/>
       <c r="E172" s="15">
         <f t="shared" si="24"/>
-        <v>0.99019607843137292</v>
+        <v>0.98850574712643657</v>
       </c>
       <c r="F172" s="15">
         <f t="shared" si="21"/>
-        <v>0.82426778242677834</v>
+        <v>0.816593886462883</v>
       </c>
       <c r="G172" s="30"/>
-      <c r="H172" s="30"/>
+      <c r="H172" s="30">
+        <v>42796</v>
+      </c>
       <c r="I172" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6792,21 +7062,23 @@
       <c r="D173" s="19"/>
       <c r="E173" s="15">
         <f t="shared" si="24"/>
-        <v>1.0000000000000004</v>
+        <v>0.99999999999999978</v>
       </c>
       <c r="F173" s="15">
         <f t="shared" si="21"/>
-        <v>0.82705718270571837</v>
+        <v>0.81950509461426579</v>
       </c>
       <c r="G173" s="30"/>
-      <c r="H173" s="30"/>
-      <c r="I173" s="9" t="str">
+      <c r="H173" s="30">
+        <v>42796</v>
+      </c>
+      <c r="I173" s="9">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="J173" s="38" t="str">
+        <v>51</v>
+      </c>
+      <c r="J173" s="38">
         <f t="shared" si="23"/>
-        <v/>
+        <v>0.85</v>
       </c>
     </row>
     <row r="174" spans="1:10" ht="21" thickBot="1">
@@ -6822,7 +7094,7 @@
       <c r="E174" s="27"/>
       <c r="F174" s="29">
         <f t="shared" si="21"/>
-        <v>0.82705718270571837</v>
+        <v>0.81950509461426579</v>
       </c>
       <c r="G174" s="41" t="str">
         <f>IF(COUNTA(G175:G191)=COUNTA(B175:B191), "COMPLETE", "")</f>
@@ -6854,10 +7126,12 @@
       </c>
       <c r="F175" s="15">
         <f t="shared" si="21"/>
-        <v>0.83542538354253848</v>
+        <v>0.82823871906841429</v>
       </c>
       <c r="G175" s="30"/>
-      <c r="H175" s="30"/>
+      <c r="H175" s="30">
+        <v>42797</v>
+      </c>
       <c r="I175" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6881,10 +7155,12 @@
       </c>
       <c r="F176" s="15">
         <f t="shared" si="21"/>
-        <v>0.84518828451882855</v>
+        <v>0.83842794759825412</v>
       </c>
       <c r="G176" s="30"/>
-      <c r="H176" s="30"/>
+      <c r="H176" s="30">
+        <v>42797</v>
+      </c>
       <c r="I176" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6908,10 +7184,12 @@
       </c>
       <c r="F177" s="15">
         <f t="shared" si="21"/>
-        <v>0.85076708507670862</v>
+        <v>0.84425036390101982</v>
       </c>
       <c r="G177" s="30"/>
-      <c r="H177" s="30"/>
+      <c r="H177" s="30">
+        <v>42797</v>
+      </c>
       <c r="I177" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6935,10 +7213,12 @@
       </c>
       <c r="F178" s="15">
         <f t="shared" si="21"/>
-        <v>0.86331938633193872</v>
+        <v>0.85735080058224256</v>
       </c>
       <c r="G178" s="30"/>
-      <c r="H178" s="30"/>
+      <c r="H178" s="30">
+        <v>42797</v>
+      </c>
       <c r="I178" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6962,10 +7242,12 @@
       </c>
       <c r="F179" s="15">
         <f t="shared" si="21"/>
-        <v>0.86750348675034872</v>
+        <v>0.8617176128093168</v>
       </c>
       <c r="G179" s="30"/>
-      <c r="H179" s="30"/>
+      <c r="H179" s="30">
+        <v>42797</v>
+      </c>
       <c r="I179" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6989,10 +7271,12 @@
       </c>
       <c r="F180" s="15">
         <f t="shared" si="21"/>
-        <v>0.87029288702928875</v>
+        <v>0.8646288209606996</v>
       </c>
       <c r="G180" s="30"/>
-      <c r="H180" s="30"/>
+      <c r="H180" s="30">
+        <v>42797</v>
+      </c>
       <c r="I180" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7016,10 +7300,12 @@
       </c>
       <c r="F181" s="15">
         <f t="shared" si="21"/>
-        <v>0.87447698744769875</v>
+        <v>0.86899563318777384</v>
       </c>
       <c r="G181" s="30"/>
-      <c r="H181" s="30"/>
+      <c r="H181" s="30">
+        <v>42797</v>
+      </c>
       <c r="I181" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7043,10 +7329,12 @@
       </c>
       <c r="F182" s="15">
         <f t="shared" si="21"/>
-        <v>0.88284518828451886</v>
+        <v>0.87772925764192233</v>
       </c>
       <c r="G182" s="30"/>
-      <c r="H182" s="30"/>
+      <c r="H182" s="30">
+        <v>42797</v>
+      </c>
       <c r="I182" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7070,10 +7358,12 @@
       </c>
       <c r="F183" s="15">
         <f t="shared" si="21"/>
-        <v>0.89958158995815907</v>
+        <v>0.89519650655021932</v>
       </c>
       <c r="G183" s="30"/>
-      <c r="H183" s="30"/>
+      <c r="H183" s="30">
+        <v>42797</v>
+      </c>
       <c r="I183" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7097,17 +7387,19 @@
       </c>
       <c r="F184" s="15">
         <f t="shared" si="21"/>
-        <v>0.91073919107391921</v>
+        <v>0.9068413391557506</v>
       </c>
       <c r="G184" s="30"/>
-      <c r="H184" s="30"/>
-      <c r="I184" s="9" t="str">
+      <c r="H184" s="30">
+        <v>42797</v>
+      </c>
+      <c r="I184" s="9">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="J184" s="38" t="str">
+        <v>60</v>
+      </c>
+      <c r="J184" s="38">
         <f t="shared" si="23"/>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="185" spans="1:10" outlineLevel="1">
@@ -7124,10 +7416,12 @@
       </c>
       <c r="F185" s="15">
         <f t="shared" si="21"/>
-        <v>0.93305439330543938</v>
+        <v>0.93013100436681317</v>
       </c>
       <c r="G185" s="30"/>
-      <c r="H185" s="30"/>
+      <c r="H185" s="30">
+        <v>42798</v>
+      </c>
       <c r="I185" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7151,10 +7445,12 @@
       </c>
       <c r="F186" s="15">
         <f t="shared" si="21"/>
-        <v>0.94839609483960952</v>
+        <v>0.94614264919941871</v>
       </c>
       <c r="G186" s="30"/>
-      <c r="H186" s="30"/>
+      <c r="H186" s="30">
+        <v>42798</v>
+      </c>
       <c r="I186" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7178,10 +7474,12 @@
       </c>
       <c r="F187" s="15">
         <f t="shared" si="21"/>
-        <v>0.95676429567642962</v>
+        <v>0.9548762736535672</v>
       </c>
       <c r="G187" s="30"/>
-      <c r="H187" s="30"/>
+      <c r="H187" s="30">
+        <v>42798</v>
+      </c>
       <c r="I187" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7205,10 +7503,12 @@
       </c>
       <c r="F188" s="15">
         <f t="shared" si="21"/>
-        <v>0.96094839609483962</v>
+        <v>0.95924308588064144</v>
       </c>
       <c r="G188" s="30"/>
-      <c r="H188" s="30"/>
+      <c r="H188" s="30">
+        <v>42798</v>
+      </c>
       <c r="I188" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7232,10 +7532,12 @@
       </c>
       <c r="F189" s="15">
         <f t="shared" si="21"/>
-        <v>0.96513249651324962</v>
+        <v>0.96360989810771569</v>
       </c>
       <c r="G189" s="30"/>
-      <c r="H189" s="30"/>
+      <c r="H189" s="30">
+        <v>42798</v>
+      </c>
       <c r="I189" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7259,10 +7561,12 @@
       </c>
       <c r="F190" s="15">
         <f t="shared" si="21"/>
-        <v>0.97350069735006972</v>
+        <v>0.97234352256186418</v>
       </c>
       <c r="G190" s="30"/>
-      <c r="H190" s="30"/>
+      <c r="H190" s="30">
+        <v>42798</v>
+      </c>
       <c r="I190" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7286,10 +7590,12 @@
       </c>
       <c r="F191" s="15">
         <f t="shared" si="21"/>
-        <v>0.97768479776847972</v>
+        <v>0.97671033478893843</v>
       </c>
       <c r="G191" s="30"/>
-      <c r="H191" s="30"/>
+      <c r="H191" s="30">
+        <v>42798</v>
+      </c>
       <c r="I191" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7312,7 +7618,7 @@
       <c r="E192" s="27"/>
       <c r="F192" s="29">
         <f t="shared" si="21"/>
-        <v>0.97768479776847972</v>
+        <v>0.97671033478893843</v>
       </c>
       <c r="G192" s="41" t="str">
         <f>IF(COUNTA(G193:G195)=COUNTA(B193:B195), "COMPLETE", "")</f>
@@ -7344,10 +7650,12 @@
       </c>
       <c r="F193" s="15">
         <f t="shared" si="21"/>
-        <v>0.98744769874476979</v>
+        <v>0.98689956331877826</v>
       </c>
       <c r="G193" s="30"/>
-      <c r="H193" s="30"/>
+      <c r="H193" s="30">
+        <v>42798</v>
+      </c>
       <c r="I193" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7371,10 +7679,12 @@
       </c>
       <c r="F194" s="15">
         <f t="shared" si="21"/>
-        <v>0.99581589958158989</v>
+        <v>0.99563318777292675</v>
       </c>
       <c r="G194" s="30"/>
-      <c r="H194" s="30"/>
+      <c r="H194" s="30">
+        <v>42798</v>
+      </c>
       <c r="I194" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7398,17 +7708,19 @@
       </c>
       <c r="F195" s="15">
         <f t="shared" si="21"/>
-        <v>0.99999999999999989</v>
+        <v>1.0000000000000009</v>
       </c>
       <c r="G195" s="30"/>
-      <c r="H195" s="30"/>
-      <c r="I195" s="9" t="str">
+      <c r="H195" s="30">
+        <v>42798</v>
+      </c>
+      <c r="I195" s="9">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="J195" s="38" t="str">
+        <v>64</v>
+      </c>
+      <c r="J195" s="38">
         <f t="shared" si="23"/>
-        <v/>
+        <v>1.0666666666666667</v>
       </c>
     </row>
     <row r="197" spans="2:10" ht="15.75" thickBot="1">
@@ -7417,7 +7729,7 @@
       </c>
       <c r="C197" s="40">
         <f>SUM(C4:C196)</f>
-        <v>717</v>
+        <v>687</v>
       </c>
     </row>
     <row r="198" spans="2:10" ht="15.75" thickTop="1">
@@ -7426,7 +7738,7 @@
       </c>
       <c r="C198" s="12">
         <f>+C197/60</f>
-        <v>11.95</v>
+        <v>11.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
progress on section 6
</commit_message>
<xml_diff>
--- a/Ultimate Excel Programmer - VBA (Udemy) - Video Listing.xlsx
+++ b/Ultimate Excel Programmer - VBA (Udemy) - Video Listing.xlsx
@@ -7,11 +7,11 @@
     <workbookView xWindow="615" yWindow="225" windowWidth="22425" windowHeight="14745"/>
   </bookViews>
   <sheets>
-    <sheet name="Unity Course Video Listing" sheetId="1" r:id="rId1"/>
+    <sheet name="Excel VBA Course Video Listing" sheetId="1" r:id="rId1"/>
     <sheet name="Orig Data" sheetId="4" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Unity Course Video Listing'!$3:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Excel VBA Course Video Listing'!$3:$3</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="251">
   <si>
     <t>VIDEO NAME</t>
   </si>
@@ -1130,6 +1130,9 @@
   </si>
   <si>
     <t>130. Compliance Checker for your Forms or Quizzes Part 1   3:36</t>
+  </si>
+  <si>
+    <t>on hold until after Unity exam</t>
   </si>
 </sst>
 </file>
@@ -1975,11 +1978,11 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J198"/>
+  <dimension ref="A1:K198"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A53" sqref="A53"/>
+      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -2007,7 +2010,7 @@
       </c>
       <c r="F1" s="34">
         <f>SUMIF(G4:G196, "&gt;0", C4:C196)</f>
-        <v>140</v>
+        <v>177</v>
       </c>
       <c r="G1" s="35">
         <f>+C197</f>
@@ -2015,7 +2018,7 @@
       </c>
       <c r="H1" s="36">
         <f>+F1/G1</f>
-        <v>0.20378457059679767</v>
+        <v>0.2576419213973799</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -3436,7 +3439,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:10" outlineLevel="1">
+    <row r="49" spans="1:11" outlineLevel="1">
       <c r="B49" s="18" t="s">
         <v>65</v>
       </c>
@@ -3467,7 +3470,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:10" outlineLevel="1">
+    <row r="50" spans="1:11" outlineLevel="1">
       <c r="B50" s="18" t="s">
         <v>66</v>
       </c>
@@ -3498,7 +3501,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:10" outlineLevel="1">
+    <row r="51" spans="1:11" outlineLevel="1">
       <c r="B51" s="18" t="s">
         <v>67</v>
       </c>
@@ -3529,7 +3532,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:10" outlineLevel="1">
+    <row r="52" spans="1:11" outlineLevel="1">
       <c r="B52" s="18" t="s">
         <v>68</v>
       </c>
@@ -3560,7 +3563,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="53" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="B53" s="18" t="s">
         <v>69</v>
       </c>
@@ -3582,16 +3585,19 @@
       <c r="H53" s="30">
         <v>42788</v>
       </c>
-      <c r="I53" s="9" t="str">
+      <c r="I53" s="9">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J53" s="38" t="str">
+        <v>34</v>
+      </c>
+      <c r="J53" s="38">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="21" thickBot="1">
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="K53" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="21" thickBot="1">
       <c r="A54" s="28" t="s">
         <v>235</v>
       </c>
@@ -3619,7 +3625,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="55" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
       <c r="B55" s="18" t="s">
         <v>72</v>
       </c>
@@ -3638,9 +3644,11 @@
         <f t="shared" si="6"/>
         <v>0.20815138282387188</v>
       </c>
-      <c r="G55" s="30"/>
+      <c r="G55" s="30">
+        <v>42871</v>
+      </c>
       <c r="H55" s="30">
-        <v>42788</v>
+        <v>42871</v>
       </c>
       <c r="I55" s="9" t="str">
         <f t="shared" si="7"/>
@@ -3651,7 +3659,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:10" outlineLevel="1">
+    <row r="56" spans="1:11" outlineLevel="1">
       <c r="B56" s="18" t="s">
         <v>73</v>
       </c>
@@ -3667,9 +3675,11 @@
         <f t="shared" si="6"/>
         <v>0.21251819505094613</v>
       </c>
-      <c r="G56" s="30"/>
+      <c r="G56" s="30">
+        <v>42871</v>
+      </c>
       <c r="H56" s="30">
-        <v>42788</v>
+        <v>42871</v>
       </c>
       <c r="I56" s="9" t="str">
         <f t="shared" si="7"/>
@@ -3680,7 +3690,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:10" outlineLevel="1">
+    <row r="57" spans="1:11" outlineLevel="1">
       <c r="B57" s="18" t="s">
         <v>74</v>
       </c>
@@ -3696,9 +3706,11 @@
         <f t="shared" si="6"/>
         <v>0.21397379912663755</v>
       </c>
-      <c r="G57" s="30"/>
+      <c r="G57" s="30">
+        <v>42871</v>
+      </c>
       <c r="H57" s="30">
-        <v>42788</v>
+        <v>42871</v>
       </c>
       <c r="I57" s="9" t="str">
         <f t="shared" si="7"/>
@@ -3709,7 +3721,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:10" outlineLevel="1">
+    <row r="58" spans="1:11" outlineLevel="1">
       <c r="B58" s="18" t="s">
         <v>75</v>
       </c>
@@ -3725,9 +3737,11 @@
         <f t="shared" si="6"/>
         <v>0.2197962154294032</v>
       </c>
-      <c r="G58" s="30"/>
+      <c r="G58" s="30">
+        <v>42871</v>
+      </c>
       <c r="H58" s="30">
-        <v>42788</v>
+        <v>42871</v>
       </c>
       <c r="I58" s="9" t="str">
         <f t="shared" si="7"/>
@@ -3738,7 +3752,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:10" outlineLevel="1">
+    <row r="59" spans="1:11" outlineLevel="1">
       <c r="B59" s="18" t="s">
         <v>76</v>
       </c>
@@ -3754,9 +3768,11 @@
         <f t="shared" si="6"/>
         <v>0.22852983988355166</v>
       </c>
-      <c r="G59" s="30"/>
+      <c r="G59" s="30">
+        <v>42871</v>
+      </c>
       <c r="H59" s="30">
-        <v>42788</v>
+        <v>42871</v>
       </c>
       <c r="I59" s="9" t="str">
         <f t="shared" si="7"/>
@@ -3767,7 +3783,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:10" outlineLevel="1">
+    <row r="60" spans="1:11" outlineLevel="1">
       <c r="B60" s="18" t="s">
         <v>78</v>
       </c>
@@ -3783,20 +3799,22 @@
         <f t="shared" si="6"/>
         <v>0.2343522561863173</v>
       </c>
-      <c r="G60" s="30"/>
+      <c r="G60" s="30">
+        <v>42871</v>
+      </c>
       <c r="H60" s="30">
-        <v>42788</v>
-      </c>
-      <c r="I60" s="9" t="str">
+        <v>42871</v>
+      </c>
+      <c r="I60" s="9">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J60" s="38" t="str">
+        <v>21</v>
+      </c>
+      <c r="J60" s="38">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:10" outlineLevel="1">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" outlineLevel="1">
       <c r="B61" s="18" t="s">
         <v>79</v>
       </c>
@@ -3812,9 +3830,11 @@
         <f t="shared" si="6"/>
         <v>0.23871906841339155</v>
       </c>
-      <c r="G61" s="30"/>
+      <c r="G61" s="30">
+        <v>42896</v>
+      </c>
       <c r="H61" s="30">
-        <v>42788</v>
+        <v>42896</v>
       </c>
       <c r="I61" s="9" t="str">
         <f t="shared" si="7"/>
@@ -3825,7 +3845,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:10" outlineLevel="1">
+    <row r="62" spans="1:11" outlineLevel="1">
       <c r="B62" s="18" t="s">
         <v>80</v>
       </c>
@@ -3841,20 +3861,22 @@
         <f t="shared" si="6"/>
         <v>0.24017467248908297</v>
       </c>
-      <c r="G62" s="30"/>
+      <c r="G62" s="30">
+        <v>42896</v>
+      </c>
       <c r="H62" s="30">
-        <v>42788</v>
-      </c>
-      <c r="I62" s="9">
+        <v>42896</v>
+      </c>
+      <c r="I62" s="9" t="str">
         <f t="shared" si="7"/>
-        <v>59</v>
-      </c>
-      <c r="J62" s="38">
+        <v/>
+      </c>
+      <c r="J62" s="38" t="str">
         <f t="shared" si="8"/>
-        <v>0.98333333333333328</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" outlineLevel="1">
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:11" outlineLevel="1">
       <c r="B63" s="18" t="s">
         <v>82</v>
       </c>
@@ -3870,9 +3892,11 @@
         <f t="shared" si="6"/>
         <v>0.24454148471615722</v>
       </c>
-      <c r="G63" s="30"/>
+      <c r="G63" s="30">
+        <v>42896</v>
+      </c>
       <c r="H63" s="30">
-        <v>42790</v>
+        <v>42896</v>
       </c>
       <c r="I63" s="9" t="str">
         <f t="shared" si="7"/>
@@ -3883,7 +3907,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:10" outlineLevel="1">
+    <row r="64" spans="1:11" outlineLevel="1">
       <c r="B64" s="18" t="s">
         <v>83</v>
       </c>
@@ -3899,9 +3923,11 @@
         <f t="shared" si="6"/>
         <v>0.24599708879184864</v>
       </c>
-      <c r="G64" s="30"/>
+      <c r="G64" s="30">
+        <v>42896</v>
+      </c>
       <c r="H64" s="30">
-        <v>42790</v>
+        <v>42896</v>
       </c>
       <c r="I64" s="9" t="str">
         <f t="shared" si="7"/>
@@ -3928,9 +3954,11 @@
         <f t="shared" si="6"/>
         <v>0.24745269286754007</v>
       </c>
-      <c r="G65" s="30"/>
+      <c r="G65" s="30">
+        <v>42896</v>
+      </c>
       <c r="H65" s="30">
-        <v>42790</v>
+        <v>42896</v>
       </c>
       <c r="I65" s="9" t="str">
         <f t="shared" si="7"/>
@@ -3957,9 +3985,11 @@
         <f t="shared" si="6"/>
         <v>0.25036390101892292</v>
       </c>
-      <c r="G66" s="30"/>
+      <c r="G66" s="30">
+        <v>42896</v>
+      </c>
       <c r="H66" s="30">
-        <v>42790</v>
+        <v>42896</v>
       </c>
       <c r="I66" s="9" t="str">
         <f t="shared" si="7"/>
@@ -3986,9 +4016,11 @@
         <f t="shared" si="6"/>
         <v>0.25327510917030577</v>
       </c>
-      <c r="G67" s="30"/>
+      <c r="G67" s="30">
+        <v>42896</v>
+      </c>
       <c r="H67" s="30">
-        <v>42790</v>
+        <v>42896</v>
       </c>
       <c r="I67" s="9" t="str">
         <f t="shared" si="7"/>
@@ -4015,9 +4047,11 @@
         <f t="shared" si="6"/>
         <v>0.25764192139738001</v>
       </c>
-      <c r="G68" s="30"/>
+      <c r="G68" s="30">
+        <v>42896</v>
+      </c>
       <c r="H68" s="30">
-        <v>42790</v>
+        <v>42896</v>
       </c>
       <c r="I68" s="9" t="str">
         <f t="shared" si="7"/>
@@ -4046,7 +4080,7 @@
       </c>
       <c r="G69" s="30"/>
       <c r="H69" s="30">
-        <v>42790</v>
+        <v>42896</v>
       </c>
       <c r="I69" s="9" t="str">
         <f t="shared" si="7"/>
@@ -4075,7 +4109,7 @@
       </c>
       <c r="G70" s="30"/>
       <c r="H70" s="30">
-        <v>42790</v>
+        <v>42896</v>
       </c>
       <c r="I70" s="9" t="str">
         <f t="shared" si="7"/>
@@ -4104,7 +4138,7 @@
       </c>
       <c r="G71" s="30"/>
       <c r="H71" s="30">
-        <v>42790</v>
+        <v>42896</v>
       </c>
       <c r="I71" s="9" t="str">
         <f t="shared" si="7"/>
@@ -4133,7 +4167,7 @@
       </c>
       <c r="G72" s="30"/>
       <c r="H72" s="30">
-        <v>42790</v>
+        <v>42896</v>
       </c>
       <c r="I72" s="9" t="str">
         <f t="shared" ref="I72:I135" si="15">IF(H72="", "", IF(ISBLANK(H73), IF(H72&lt;&gt;H74, SUMIF(H:H,H72,C:C), ""), IF(H72&lt;&gt;H73, SUMIF(H:H,H72,C:C), "")))</f>
@@ -4162,7 +4196,7 @@
       </c>
       <c r="G73" s="30"/>
       <c r="H73" s="30">
-        <v>42790</v>
+        <v>42896</v>
       </c>
       <c r="I73" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4191,7 +4225,7 @@
       </c>
       <c r="G74" s="30"/>
       <c r="H74" s="30">
-        <v>42790</v>
+        <v>42896</v>
       </c>
       <c r="I74" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4220,7 +4254,7 @@
       </c>
       <c r="G75" s="30"/>
       <c r="H75" s="30">
-        <v>42790</v>
+        <v>42896</v>
       </c>
       <c r="I75" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4249,15 +4283,15 @@
       </c>
       <c r="G76" s="30"/>
       <c r="H76" s="30">
-        <v>42790</v>
+        <v>42896</v>
       </c>
       <c r="I76" s="9">
         <f t="shared" si="15"/>
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="J76" s="38">
         <f t="shared" si="16"/>
-        <v>1.0833333333333333</v>
+        <v>1.1499999999999999</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="21" thickBot="1">
@@ -4309,7 +4343,7 @@
       </c>
       <c r="G78" s="30"/>
       <c r="H78" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I78" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4338,7 +4372,7 @@
       </c>
       <c r="G79" s="30"/>
       <c r="H79" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I79" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4367,7 +4401,7 @@
       </c>
       <c r="G80" s="30"/>
       <c r="H80" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I80" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4396,7 +4430,7 @@
       </c>
       <c r="G81" s="30"/>
       <c r="H81" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I81" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4425,7 +4459,7 @@
       </c>
       <c r="G82" s="30"/>
       <c r="H82" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I82" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4454,7 +4488,7 @@
       </c>
       <c r="G83" s="30"/>
       <c r="H83" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I83" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4483,7 +4517,7 @@
       </c>
       <c r="G84" s="30"/>
       <c r="H84" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I84" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4512,7 +4546,7 @@
       </c>
       <c r="G85" s="30"/>
       <c r="H85" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I85" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4541,7 +4575,7 @@
       </c>
       <c r="G86" s="30"/>
       <c r="H86" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I86" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4570,7 +4604,7 @@
       </c>
       <c r="G87" s="30"/>
       <c r="H87" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I87" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4599,7 +4633,7 @@
       </c>
       <c r="G88" s="30"/>
       <c r="H88" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I88" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4628,7 +4662,7 @@
       </c>
       <c r="G89" s="30"/>
       <c r="H89" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I89" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4657,7 +4691,7 @@
       </c>
       <c r="G90" s="30"/>
       <c r="H90" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I90" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4686,7 +4720,7 @@
       </c>
       <c r="G91" s="30"/>
       <c r="H91" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I91" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4715,7 +4749,7 @@
       </c>
       <c r="G92" s="30"/>
       <c r="H92" s="30">
-        <v>42791</v>
+        <v>42897</v>
       </c>
       <c r="I92" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4744,15 +4778,15 @@
       </c>
       <c r="G93" s="30"/>
       <c r="H93" s="30">
-        <v>42791</v>
-      </c>
-      <c r="I93" s="9">
+        <v>42897</v>
+      </c>
+      <c r="I93" s="9" t="str">
         <f t="shared" si="15"/>
-        <v>57</v>
-      </c>
-      <c r="J93" s="38">
+        <v/>
+      </c>
+      <c r="J93" s="38" t="str">
         <f t="shared" si="16"/>
-        <v>0.95</v>
+        <v/>
       </c>
     </row>
     <row r="94" spans="2:10" outlineLevel="1">
@@ -4773,7 +4807,7 @@
       </c>
       <c r="G94" s="30"/>
       <c r="H94" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I94" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4802,7 +4836,7 @@
       </c>
       <c r="G95" s="30"/>
       <c r="H95" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I95" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4831,7 +4865,7 @@
       </c>
       <c r="G96" s="30"/>
       <c r="H96" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I96" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4860,7 +4894,7 @@
       </c>
       <c r="G97" s="30"/>
       <c r="H97" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I97" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4889,7 +4923,7 @@
       </c>
       <c r="G98" s="30"/>
       <c r="H98" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I98" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4918,7 +4952,7 @@
       </c>
       <c r="G99" s="30"/>
       <c r="H99" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I99" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4947,7 +4981,7 @@
       </c>
       <c r="G100" s="30"/>
       <c r="H100" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I100" s="9" t="str">
         <f t="shared" si="15"/>
@@ -4976,7 +5010,7 @@
       </c>
       <c r="G101" s="30"/>
       <c r="H101" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I101" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5036,7 +5070,7 @@
       </c>
       <c r="G103" s="30"/>
       <c r="H103" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I103" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5065,7 +5099,7 @@
       </c>
       <c r="G104" s="30"/>
       <c r="H104" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I104" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5094,7 +5128,7 @@
       </c>
       <c r="G105" s="30"/>
       <c r="H105" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I105" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5123,7 +5157,7 @@
       </c>
       <c r="G106" s="30"/>
       <c r="H106" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I106" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5152,7 +5186,7 @@
       </c>
       <c r="G107" s="30"/>
       <c r="H107" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I107" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5181,7 +5215,7 @@
       </c>
       <c r="G108" s="30"/>
       <c r="H108" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I108" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5210,7 +5244,7 @@
       </c>
       <c r="G109" s="30"/>
       <c r="H109" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I109" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5239,7 +5273,7 @@
       </c>
       <c r="G110" s="30"/>
       <c r="H110" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I110" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5268,7 +5302,7 @@
       </c>
       <c r="G111" s="30"/>
       <c r="H111" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I111" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5297,7 +5331,7 @@
       </c>
       <c r="G112" s="30"/>
       <c r="H112" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I112" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5326,7 +5360,7 @@
       </c>
       <c r="G113" s="30"/>
       <c r="H113" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I113" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5355,7 +5389,7 @@
       </c>
       <c r="G114" s="30"/>
       <c r="H114" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I114" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5384,7 +5418,7 @@
       </c>
       <c r="G115" s="30"/>
       <c r="H115" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I115" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5413,15 +5447,15 @@
       </c>
       <c r="G116" s="30"/>
       <c r="H116" s="30">
-        <v>42792</v>
+        <v>42897</v>
       </c>
       <c r="I116" s="9">
         <f t="shared" si="15"/>
-        <v>62</v>
+        <v>119</v>
       </c>
       <c r="J116" s="38">
         <f t="shared" si="16"/>
-        <v>1.0333333333333334</v>
+        <v>1.9833333333333334</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="21" thickBot="1">
@@ -5473,7 +5507,7 @@
       </c>
       <c r="G118" s="30"/>
       <c r="H118" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I118" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5502,7 +5536,7 @@
       </c>
       <c r="G119" s="30"/>
       <c r="H119" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I119" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5531,7 +5565,7 @@
       </c>
       <c r="G120" s="30"/>
       <c r="H120" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I120" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5560,7 +5594,7 @@
       </c>
       <c r="G121" s="30"/>
       <c r="H121" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I121" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5589,7 +5623,7 @@
       </c>
       <c r="G122" s="30"/>
       <c r="H122" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I122" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5618,7 +5652,7 @@
       </c>
       <c r="G123" s="30"/>
       <c r="H123" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I123" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5647,7 +5681,7 @@
       </c>
       <c r="G124" s="30"/>
       <c r="H124" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I124" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5676,7 +5710,7 @@
       </c>
       <c r="G125" s="30"/>
       <c r="H125" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I125" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5705,7 +5739,7 @@
       </c>
       <c r="G126" s="30"/>
       <c r="H126" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I126" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5734,7 +5768,7 @@
       </c>
       <c r="G127" s="30"/>
       <c r="H127" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I127" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5763,7 +5797,7 @@
       </c>
       <c r="G128" s="30"/>
       <c r="H128" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I128" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5792,7 +5826,7 @@
       </c>
       <c r="G129" s="30"/>
       <c r="H129" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I129" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5821,7 +5855,7 @@
       </c>
       <c r="G130" s="30"/>
       <c r="H130" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I130" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5850,7 +5884,7 @@
       </c>
       <c r="G131" s="30"/>
       <c r="H131" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I131" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5879,7 +5913,7 @@
       </c>
       <c r="G132" s="30"/>
       <c r="H132" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I132" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5908,7 +5942,7 @@
       </c>
       <c r="G133" s="30"/>
       <c r="H133" s="30">
-        <v>42793</v>
+        <v>42898</v>
       </c>
       <c r="I133" s="9" t="str">
         <f t="shared" si="15"/>
@@ -5937,15 +5971,15 @@
       </c>
       <c r="G134" s="30"/>
       <c r="H134" s="30">
-        <v>42793</v>
-      </c>
-      <c r="I134" s="9">
+        <v>42898</v>
+      </c>
+      <c r="I134" s="9" t="str">
         <f t="shared" si="15"/>
-        <v>40</v>
-      </c>
-      <c r="J134" s="38">
+        <v/>
+      </c>
+      <c r="J134" s="38" t="str">
         <f t="shared" si="16"/>
-        <v>0.66666666666666663</v>
+        <v/>
       </c>
     </row>
     <row r="135" spans="1:10" ht="21" thickBot="1">
@@ -5997,7 +6031,7 @@
       </c>
       <c r="G136" s="30"/>
       <c r="H136" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I136" s="9" t="str">
         <f t="shared" ref="I136:I195" si="22">IF(H136="", "", IF(ISBLANK(H137), IF(H136&lt;&gt;H138, SUMIF(H:H,H136,C:C), ""), IF(H136&lt;&gt;H137, SUMIF(H:H,H136,C:C), "")))</f>
@@ -6026,7 +6060,7 @@
       </c>
       <c r="G137" s="30"/>
       <c r="H137" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I137" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6055,7 +6089,7 @@
       </c>
       <c r="G138" s="30"/>
       <c r="H138" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I138" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6084,7 +6118,7 @@
       </c>
       <c r="G139" s="30"/>
       <c r="H139" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I139" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6113,7 +6147,7 @@
       </c>
       <c r="G140" s="30"/>
       <c r="H140" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I140" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6142,7 +6176,7 @@
       </c>
       <c r="G141" s="30"/>
       <c r="H141" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I141" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6171,7 +6205,7 @@
       </c>
       <c r="G142" s="30"/>
       <c r="H142" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I142" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6200,7 +6234,7 @@
       </c>
       <c r="G143" s="30"/>
       <c r="H143" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I143" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6229,7 +6263,7 @@
       </c>
       <c r="G144" s="30"/>
       <c r="H144" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I144" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6258,7 +6292,7 @@
       </c>
       <c r="G145" s="30"/>
       <c r="H145" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I145" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6287,7 +6321,7 @@
       </c>
       <c r="G146" s="30"/>
       <c r="H146" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I146" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6316,7 +6350,7 @@
       </c>
       <c r="G147" s="30"/>
       <c r="H147" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I147" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6345,7 +6379,7 @@
       </c>
       <c r="G148" s="30"/>
       <c r="H148" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I148" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6374,7 +6408,7 @@
       </c>
       <c r="G149" s="30"/>
       <c r="H149" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I149" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6403,7 +6437,7 @@
       </c>
       <c r="G150" s="30"/>
       <c r="H150" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I150" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6432,7 +6466,7 @@
       </c>
       <c r="G151" s="30"/>
       <c r="H151" s="30">
-        <v>42794</v>
+        <v>42898</v>
       </c>
       <c r="I151" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6461,15 +6495,15 @@
       </c>
       <c r="G152" s="30"/>
       <c r="H152" s="30">
-        <v>42794</v>
-      </c>
-      <c r="I152" s="9">
+        <v>42898</v>
+      </c>
+      <c r="I152" s="9" t="str">
         <f t="shared" si="22"/>
-        <v>65</v>
-      </c>
-      <c r="J152" s="38">
+        <v/>
+      </c>
+      <c r="J152" s="38" t="str">
         <f t="shared" si="23"/>
-        <v>1.0833333333333333</v>
+        <v/>
       </c>
     </row>
     <row r="153" spans="2:10" outlineLevel="1">
@@ -6490,7 +6524,7 @@
       </c>
       <c r="G153" s="30"/>
       <c r="H153" s="30">
-        <v>42795</v>
+        <v>42898</v>
       </c>
       <c r="I153" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6519,7 +6553,7 @@
       </c>
       <c r="G154" s="30"/>
       <c r="H154" s="30">
-        <v>42795</v>
+        <v>42898</v>
       </c>
       <c r="I154" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6548,7 +6582,7 @@
       </c>
       <c r="G155" s="30"/>
       <c r="H155" s="30">
-        <v>42795</v>
+        <v>42898</v>
       </c>
       <c r="I155" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6577,7 +6611,7 @@
       </c>
       <c r="G156" s="30"/>
       <c r="H156" s="30">
-        <v>42795</v>
+        <v>42898</v>
       </c>
       <c r="I156" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6606,7 +6640,7 @@
       </c>
       <c r="G157" s="30"/>
       <c r="H157" s="30">
-        <v>42795</v>
+        <v>42898</v>
       </c>
       <c r="I157" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6635,7 +6669,7 @@
       </c>
       <c r="G158" s="30"/>
       <c r="H158" s="30">
-        <v>42795</v>
+        <v>42898</v>
       </c>
       <c r="I158" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6664,7 +6698,7 @@
       </c>
       <c r="G159" s="30"/>
       <c r="H159" s="30">
-        <v>42795</v>
+        <v>42898</v>
       </c>
       <c r="I159" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6693,7 +6727,7 @@
       </c>
       <c r="G160" s="30"/>
       <c r="H160" s="30">
-        <v>42795</v>
+        <v>42898</v>
       </c>
       <c r="I160" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6722,7 +6756,7 @@
       </c>
       <c r="G161" s="30"/>
       <c r="H161" s="30">
-        <v>42795</v>
+        <v>42898</v>
       </c>
       <c r="I161" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6751,7 +6785,7 @@
       </c>
       <c r="G162" s="30"/>
       <c r="H162" s="30">
-        <v>42795</v>
+        <v>42898</v>
       </c>
       <c r="I162" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6780,15 +6814,15 @@
       </c>
       <c r="G163" s="30"/>
       <c r="H163" s="30">
-        <v>42795</v>
-      </c>
-      <c r="I163" s="9">
+        <v>42898</v>
+      </c>
+      <c r="I163" s="9" t="str">
         <f t="shared" si="22"/>
-        <v>58</v>
-      </c>
-      <c r="J163" s="38">
+        <v/>
+      </c>
+      <c r="J163" s="38" t="str">
         <f t="shared" si="23"/>
-        <v>0.96666666666666667</v>
+        <v/>
       </c>
     </row>
     <row r="164" spans="1:10" outlineLevel="1">
@@ -6809,7 +6843,7 @@
       </c>
       <c r="G164" s="30"/>
       <c r="H164" s="30">
-        <v>42796</v>
+        <v>42898</v>
       </c>
       <c r="I164" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6838,7 +6872,7 @@
       </c>
       <c r="G165" s="30"/>
       <c r="H165" s="30">
-        <v>42796</v>
+        <v>42898</v>
       </c>
       <c r="I165" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6867,7 +6901,7 @@
       </c>
       <c r="G166" s="30"/>
       <c r="H166" s="30">
-        <v>42796</v>
+        <v>42898</v>
       </c>
       <c r="I166" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6896,7 +6930,7 @@
       </c>
       <c r="G167" s="30"/>
       <c r="H167" s="30">
-        <v>42796</v>
+        <v>42898</v>
       </c>
       <c r="I167" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6925,7 +6959,7 @@
       </c>
       <c r="G168" s="30"/>
       <c r="H168" s="30">
-        <v>42796</v>
+        <v>42898</v>
       </c>
       <c r="I168" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6954,7 +6988,7 @@
       </c>
       <c r="G169" s="30"/>
       <c r="H169" s="30">
-        <v>42796</v>
+        <v>42898</v>
       </c>
       <c r="I169" s="9" t="str">
         <f t="shared" si="22"/>
@@ -6983,7 +7017,7 @@
       </c>
       <c r="G170" s="30"/>
       <c r="H170" s="30">
-        <v>42796</v>
+        <v>42898</v>
       </c>
       <c r="I170" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7012,7 +7046,7 @@
       </c>
       <c r="G171" s="30"/>
       <c r="H171" s="30">
-        <v>42796</v>
+        <v>42898</v>
       </c>
       <c r="I171" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7041,7 +7075,7 @@
       </c>
       <c r="G172" s="30"/>
       <c r="H172" s="30">
-        <v>42796</v>
+        <v>42898</v>
       </c>
       <c r="I172" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7070,15 +7104,15 @@
       </c>
       <c r="G173" s="30"/>
       <c r="H173" s="30">
-        <v>42796</v>
+        <v>42898</v>
       </c>
       <c r="I173" s="9">
         <f t="shared" si="22"/>
-        <v>51</v>
+        <v>214</v>
       </c>
       <c r="J173" s="38">
         <f t="shared" si="23"/>
-        <v>0.85</v>
+        <v>3.5666666666666669</v>
       </c>
     </row>
     <row r="174" spans="1:10" ht="21" thickBot="1">
@@ -7130,7 +7164,7 @@
       </c>
       <c r="G175" s="30"/>
       <c r="H175" s="30">
-        <v>42797</v>
+        <v>42899</v>
       </c>
       <c r="I175" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7159,7 +7193,7 @@
       </c>
       <c r="G176" s="30"/>
       <c r="H176" s="30">
-        <v>42797</v>
+        <v>42899</v>
       </c>
       <c r="I176" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7188,7 +7222,7 @@
       </c>
       <c r="G177" s="30"/>
       <c r="H177" s="30">
-        <v>42797</v>
+        <v>42899</v>
       </c>
       <c r="I177" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7217,7 +7251,7 @@
       </c>
       <c r="G178" s="30"/>
       <c r="H178" s="30">
-        <v>42797</v>
+        <v>42899</v>
       </c>
       <c r="I178" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7246,7 +7280,7 @@
       </c>
       <c r="G179" s="30"/>
       <c r="H179" s="30">
-        <v>42797</v>
+        <v>42899</v>
       </c>
       <c r="I179" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7275,7 +7309,7 @@
       </c>
       <c r="G180" s="30"/>
       <c r="H180" s="30">
-        <v>42797</v>
+        <v>42899</v>
       </c>
       <c r="I180" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7304,7 +7338,7 @@
       </c>
       <c r="G181" s="30"/>
       <c r="H181" s="30">
-        <v>42797</v>
+        <v>42899</v>
       </c>
       <c r="I181" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7333,7 +7367,7 @@
       </c>
       <c r="G182" s="30"/>
       <c r="H182" s="30">
-        <v>42797</v>
+        <v>42899</v>
       </c>
       <c r="I182" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7362,7 +7396,7 @@
       </c>
       <c r="G183" s="30"/>
       <c r="H183" s="30">
-        <v>42797</v>
+        <v>42899</v>
       </c>
       <c r="I183" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7391,15 +7425,15 @@
       </c>
       <c r="G184" s="30"/>
       <c r="H184" s="30">
-        <v>42797</v>
-      </c>
-      <c r="I184" s="9">
+        <v>42899</v>
+      </c>
+      <c r="I184" s="9" t="str">
         <f t="shared" si="22"/>
-        <v>60</v>
-      </c>
-      <c r="J184" s="38">
+        <v/>
+      </c>
+      <c r="J184" s="38" t="str">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v/>
       </c>
     </row>
     <row r="185" spans="1:10" outlineLevel="1">
@@ -7420,7 +7454,7 @@
       </c>
       <c r="G185" s="30"/>
       <c r="H185" s="30">
-        <v>42798</v>
+        <v>42899</v>
       </c>
       <c r="I185" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7449,7 +7483,7 @@
       </c>
       <c r="G186" s="30"/>
       <c r="H186" s="30">
-        <v>42798</v>
+        <v>42899</v>
       </c>
       <c r="I186" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7478,7 +7512,7 @@
       </c>
       <c r="G187" s="30"/>
       <c r="H187" s="30">
-        <v>42798</v>
+        <v>42899</v>
       </c>
       <c r="I187" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7507,7 +7541,7 @@
       </c>
       <c r="G188" s="30"/>
       <c r="H188" s="30">
-        <v>42798</v>
+        <v>42899</v>
       </c>
       <c r="I188" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7536,7 +7570,7 @@
       </c>
       <c r="G189" s="30"/>
       <c r="H189" s="30">
-        <v>42798</v>
+        <v>42899</v>
       </c>
       <c r="I189" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7565,7 +7599,7 @@
       </c>
       <c r="G190" s="30"/>
       <c r="H190" s="30">
-        <v>42798</v>
+        <v>42899</v>
       </c>
       <c r="I190" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7594,7 +7628,7 @@
       </c>
       <c r="G191" s="30"/>
       <c r="H191" s="30">
-        <v>42798</v>
+        <v>42899</v>
       </c>
       <c r="I191" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7654,7 +7688,7 @@
       </c>
       <c r="G193" s="30"/>
       <c r="H193" s="30">
-        <v>42798</v>
+        <v>42899</v>
       </c>
       <c r="I193" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7683,7 +7717,7 @@
       </c>
       <c r="G194" s="30"/>
       <c r="H194" s="30">
-        <v>42798</v>
+        <v>42899</v>
       </c>
       <c r="I194" s="9" t="str">
         <f t="shared" si="22"/>
@@ -7712,15 +7746,15 @@
       </c>
       <c r="G195" s="30"/>
       <c r="H195" s="30">
-        <v>42798</v>
+        <v>42899</v>
       </c>
       <c r="I195" s="9">
         <f t="shared" si="22"/>
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="J195" s="38">
         <f t="shared" si="23"/>
-        <v>1.0666666666666667</v>
+        <v>2.0666666666666669</v>
       </c>
     </row>
     <row r="197" spans="2:10" ht="15.75" thickBot="1">

</xml_diff>

<commit_message>
progress on Excel VBA course
</commit_message>
<xml_diff>
--- a/Ultimate Excel Programmer - VBA (Udemy) - Video Listing.xlsx
+++ b/Ultimate Excel Programmer - VBA (Udemy) - Video Listing.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="615" yWindow="225" windowWidth="22425" windowHeight="14745"/>
+    <workbookView xWindow="620" yWindow="220" windowWidth="22420" windowHeight="14740"/>
   </bookViews>
   <sheets>
     <sheet name="Excel VBA Course Video Listing" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Excel VBA Course Video Listing'!$3:$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1143,7 +1143,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1982,20 +1982,20 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G69" sqref="G69"/>
+      <selection pane="bottomLeft" activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" outlineLevelRow="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="82.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" customWidth="1"/>
     <col min="5" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" style="37" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" style="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="26.25" customHeight="1" thickBot="1">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="F1" s="34">
         <f>SUMIF(G4:G196, "&gt;0", C4:C196)</f>
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="G1" s="35">
         <f>+C197</f>
@@ -2018,7 +2018,7 @@
       </c>
       <c r="H1" s="36">
         <f>+F1/G1</f>
-        <v>0.2576419213973799</v>
+        <v>0.26346433770014555</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -2032,7 +2032,7 @@
         <v>11.45</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45.75" thickBot="1">
+    <row r="3" spans="1:10" ht="29" thickBot="1">
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
@@ -2072,7 +2072,7 @@
         <v>COMPLETE</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="5" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B5" s="18" t="s">
         <v>12</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="16" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B16" s="18" t="s">
         <v>26</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="18" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B18" s="18" t="s">
         <v>29</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="27" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B27" s="18" t="s">
         <v>38</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="29" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B29" s="18" t="s">
         <v>41</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="34" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B34" s="18" t="s">
         <v>46</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="36" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B36" s="22" t="s">
         <v>49</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="43" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B43" s="18" t="s">
         <v>58</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="45" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B45" s="18" t="s">
         <v>61</v>
       </c>
@@ -3563,7 +3563,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="53" spans="1:11" ht="15" outlineLevel="1" thickBot="1">
       <c r="B53" s="18" t="s">
         <v>69</v>
       </c>
@@ -3625,7 +3625,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="55" spans="1:11" ht="15" outlineLevel="1" thickBot="1">
       <c r="B55" s="18" t="s">
         <v>72</v>
       </c>
@@ -4053,13 +4053,13 @@
       <c r="H68" s="30">
         <v>42896</v>
       </c>
-      <c r="I68" s="9" t="str">
+      <c r="I68" s="9">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J68" s="38" t="str">
+        <v>16</v>
+      </c>
+      <c r="J68" s="38">
         <f t="shared" si="8"/>
-        <v/>
+        <v>0.26666666666666666</v>
       </c>
     </row>
     <row r="69" spans="1:10" outlineLevel="1">
@@ -4078,9 +4078,11 @@
         <f t="shared" si="6"/>
         <v>0.26055312954876286</v>
       </c>
-      <c r="G69" s="30"/>
+      <c r="G69" s="30">
+        <v>42920</v>
+      </c>
       <c r="H69" s="30">
-        <v>42896</v>
+        <v>42920</v>
       </c>
       <c r="I69" s="9" t="str">
         <f t="shared" si="7"/>
@@ -4107,17 +4109,19 @@
         <f t="shared" si="6"/>
         <v>0.26346433770014571</v>
       </c>
-      <c r="G70" s="30"/>
+      <c r="G70" s="30">
+        <v>42920</v>
+      </c>
       <c r="H70" s="30">
-        <v>42896</v>
-      </c>
-      <c r="I70" s="9" t="str">
+        <v>42920</v>
+      </c>
+      <c r="I70" s="9">
         <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="J70" s="38" t="str">
+        <v>4</v>
+      </c>
+      <c r="J70" s="38">
         <f t="shared" si="8"/>
-        <v/>
+        <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="71" spans="1:10" outlineLevel="1">
@@ -4137,9 +4141,7 @@
         <v>0.26783114992721996</v>
       </c>
       <c r="G71" s="30"/>
-      <c r="H71" s="30">
-        <v>42896</v>
-      </c>
+      <c r="H71" s="30"/>
       <c r="I71" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -4166,9 +4168,7 @@
         <v>0.27802037845705985</v>
       </c>
       <c r="G72" s="30"/>
-      <c r="H72" s="30">
-        <v>42896</v>
-      </c>
+      <c r="H72" s="30"/>
       <c r="I72" s="9" t="str">
         <f t="shared" ref="I72:I135" si="15">IF(H72="", "", IF(ISBLANK(H73), IF(H72&lt;&gt;H74, SUMIF(H:H,H72,C:C), ""), IF(H72&lt;&gt;H73, SUMIF(H:H,H72,C:C), "")))</f>
         <v/>
@@ -4195,9 +4195,7 @@
         <v>0.28384279475982549</v>
       </c>
       <c r="G73" s="30"/>
-      <c r="H73" s="30">
-        <v>42896</v>
-      </c>
+      <c r="H73" s="30"/>
       <c r="I73" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4224,9 +4222,7 @@
         <v>0.29112081513828253</v>
       </c>
       <c r="G74" s="30"/>
-      <c r="H74" s="30">
-        <v>42896</v>
-      </c>
+      <c r="H74" s="30"/>
       <c r="I74" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4253,9 +4249,7 @@
         <v>0.32751091703056784</v>
       </c>
       <c r="G75" s="30"/>
-      <c r="H75" s="30">
-        <v>42896</v>
-      </c>
+      <c r="H75" s="30"/>
       <c r="I75" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4265,7 +4259,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="76" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B76" s="18" t="s">
         <v>95</v>
       </c>
@@ -4282,16 +4276,14 @@
         <v>0.33478893740902488</v>
       </c>
       <c r="G76" s="30"/>
-      <c r="H76" s="30">
-        <v>42896</v>
-      </c>
-      <c r="I76" s="9">
+      <c r="H76" s="30"/>
+      <c r="I76" s="9" t="str">
         <f t="shared" si="15"/>
-        <v>69</v>
-      </c>
-      <c r="J76" s="38">
+        <v/>
+      </c>
+      <c r="J76" s="38" t="str">
         <f t="shared" si="16"/>
-        <v>1.1499999999999999</v>
+        <v/>
       </c>
     </row>
     <row r="77" spans="1:10" ht="21" thickBot="1">
@@ -4322,7 +4314,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="78" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B78" s="18" t="s">
         <v>98</v>
       </c>
@@ -4992,7 +4984,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="101" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B101" s="18" t="s">
         <v>121</v>
       </c>
@@ -5049,7 +5041,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="103" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B103" s="18" t="s">
         <v>124</v>
       </c>
@@ -5429,7 +5421,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="116" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B116" s="18" t="s">
         <v>137</v>
       </c>
@@ -5486,7 +5478,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="118" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B118" s="18" t="s">
         <v>140</v>
       </c>
@@ -5953,7 +5945,7 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="134" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B134" s="18" t="s">
         <v>156</v>
       </c>
@@ -6010,7 +6002,7 @@
         <v/>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="136" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B136" s="18" t="s">
         <v>159</v>
       </c>
@@ -7086,7 +7078,7 @@
         <v/>
       </c>
     </row>
-    <row r="173" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="173" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B173" s="18" t="s">
         <v>202</v>
       </c>
@@ -7143,7 +7135,7 @@
         <v/>
       </c>
     </row>
-    <row r="175" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="175" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B175" s="18" t="s">
         <v>205</v>
       </c>
@@ -7610,7 +7602,7 @@
         <v/>
       </c>
     </row>
-    <row r="191" spans="1:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="191" spans="1:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B191" s="18" t="s">
         <v>221</v>
       </c>
@@ -7667,7 +7659,7 @@
         <v/>
       </c>
     </row>
-    <row r="193" spans="2:10" ht="15.75" outlineLevel="1" thickBot="1">
+    <row r="193" spans="2:10" ht="15" outlineLevel="1" thickBot="1">
       <c r="B193" s="18" t="s">
         <v>224</v>
       </c>
@@ -7757,7 +7749,7 @@
         <v>2.0666666666666669</v>
       </c>
     </row>
-    <row r="197" spans="2:10" ht="15.75" thickBot="1">
+    <row r="197" spans="2:10" ht="15" thickBot="1">
       <c r="B197" s="39" t="s">
         <v>8</v>
       </c>
@@ -7766,7 +7758,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="198" spans="2:10" ht="15.75" thickTop="1">
+    <row r="198" spans="2:10" ht="15" thickTop="1">
       <c r="B198" s="39" t="s">
         <v>9</v>
       </c>
@@ -7789,21 +7781,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:A219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A219"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="42" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="19.5" thickBot="1">
+    <row r="2" spans="1:1" ht="19" thickBot="1">
       <c r="A2" s="46" t="s">
         <v>11</v>
       </c>
@@ -7823,57 +7815,57 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" thickBot="1">
+    <row r="6" spans="1:1" ht="15" thickBot="1">
       <c r="A6" s="44" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" thickBot="1">
+    <row r="7" spans="1:1" ht="15" thickBot="1">
       <c r="A7" s="43" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" thickBot="1">
+    <row r="8" spans="1:1" ht="15" thickBot="1">
       <c r="A8" s="43" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" thickBot="1">
+    <row r="9" spans="1:1" ht="15" thickBot="1">
       <c r="A9" s="43" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75" thickBot="1">
+    <row r="10" spans="1:1" ht="15" thickBot="1">
       <c r="A10" s="43" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" thickBot="1">
+    <row r="11" spans="1:1" ht="15" thickBot="1">
       <c r="A11" s="43" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" thickBot="1">
+    <row r="12" spans="1:1" ht="15" thickBot="1">
       <c r="A12" s="43" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.75" thickBot="1">
+    <row r="13" spans="1:1" ht="15" thickBot="1">
       <c r="A13" s="43" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15.75" thickBot="1">
+    <row r="14" spans="1:1" ht="15" thickBot="1">
       <c r="A14" s="43" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.75" thickBot="1">
+    <row r="15" spans="1:1" ht="15" thickBot="1">
       <c r="A15" s="43" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.75" thickBot="1">
+    <row r="16" spans="1:1" ht="15" thickBot="1">
       <c r="A16" s="43" t="s">
         <v>25</v>
       </c>
@@ -7888,52 +7880,52 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="19.5" thickBot="1">
+    <row r="19" spans="1:1" ht="19" thickBot="1">
       <c r="A19" s="46" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.75" thickBot="1">
+    <row r="20" spans="1:1" ht="15" thickBot="1">
       <c r="A20" s="45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15.75" thickBot="1">
+    <row r="21" spans="1:1" ht="15" thickBot="1">
       <c r="A21" s="43" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15.75" thickBot="1">
+    <row r="22" spans="1:1" ht="15" thickBot="1">
       <c r="A22" s="43" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15.75" thickBot="1">
+    <row r="23" spans="1:1" ht="15" thickBot="1">
       <c r="A23" s="43" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15.75" thickBot="1">
+    <row r="24" spans="1:1" ht="15" thickBot="1">
       <c r="A24" s="43" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15.75" thickBot="1">
+    <row r="25" spans="1:1" ht="15" thickBot="1">
       <c r="A25" s="43" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="15.75" thickBot="1">
+    <row r="26" spans="1:1" ht="15" thickBot="1">
       <c r="A26" s="43" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="15.75" thickBot="1">
+    <row r="27" spans="1:1" ht="15" thickBot="1">
       <c r="A27" s="43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="15.75" thickBot="1">
+    <row r="28" spans="1:1" ht="15" thickBot="1">
       <c r="A28" s="43" t="s">
         <v>37</v>
       </c>
@@ -7948,32 +7940,32 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="19.5" thickBot="1">
+    <row r="31" spans="1:1" ht="19" thickBot="1">
       <c r="A31" s="46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="15.75" thickBot="1">
+    <row r="32" spans="1:1" ht="15" thickBot="1">
       <c r="A32" s="45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="15.75" thickBot="1">
+    <row r="33" spans="1:1" ht="15" thickBot="1">
       <c r="A33" s="43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="15.75" thickBot="1">
+    <row r="34" spans="1:1" ht="15" thickBot="1">
       <c r="A34" s="43" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="15.75" thickBot="1">
+    <row r="35" spans="1:1" ht="15" thickBot="1">
       <c r="A35" s="43" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="15.75" thickBot="1">
+    <row r="36" spans="1:1" ht="15" thickBot="1">
       <c r="A36" s="43" t="s">
         <v>45</v>
       </c>
@@ -7988,7 +7980,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="19.5" thickBot="1">
+    <row r="39" spans="1:1" ht="19" thickBot="1">
       <c r="A39" s="46" t="s">
         <v>48</v>
       </c>
@@ -7998,32 +7990,32 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="15.75" thickBot="1">
+    <row r="41" spans="1:1" ht="15" thickBot="1">
       <c r="A41" s="44" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="15.75" thickBot="1">
+    <row r="42" spans="1:1" ht="15" thickBot="1">
       <c r="A42" s="43" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="15.75" thickBot="1">
+    <row r="43" spans="1:1" ht="15" thickBot="1">
       <c r="A43" s="43" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="15.75" thickBot="1">
+    <row r="44" spans="1:1" ht="15" thickBot="1">
       <c r="A44" s="43" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="15.75" thickBot="1">
+    <row r="45" spans="1:1" ht="15" thickBot="1">
       <c r="A45" s="43" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="15.75" thickBot="1">
+    <row r="46" spans="1:1" ht="15" thickBot="1">
       <c r="A46" s="43" t="s">
         <v>55</v>
       </c>
@@ -8033,7 +8025,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="15.75" thickBot="1">
+    <row r="48" spans="1:1" ht="15" thickBot="1">
       <c r="A48" s="44" t="s">
         <v>57</v>
       </c>
@@ -8048,47 +8040,47 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="19.5" thickBot="1">
+    <row r="51" spans="1:1" ht="19" thickBot="1">
       <c r="A51" s="46" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="15.75" thickBot="1">
+    <row r="52" spans="1:1" ht="15" thickBot="1">
       <c r="A52" s="45" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="15.75" thickBot="1">
+    <row r="53" spans="1:1" ht="15" thickBot="1">
       <c r="A53" s="43" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="15.75" thickBot="1">
+    <row r="54" spans="1:1" ht="15" thickBot="1">
       <c r="A54" s="43" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="15.75" thickBot="1">
+    <row r="55" spans="1:1" ht="15" thickBot="1">
       <c r="A55" s="43" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="15.75" thickBot="1">
+    <row r="56" spans="1:1" ht="15" thickBot="1">
       <c r="A56" s="43" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="15.75" thickBot="1">
+    <row r="57" spans="1:1" ht="15" thickBot="1">
       <c r="A57" s="43" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="15.75" thickBot="1">
+    <row r="58" spans="1:1" ht="15" thickBot="1">
       <c r="A58" s="43" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="15.75" thickBot="1">
+    <row r="59" spans="1:1" ht="15" thickBot="1">
       <c r="A59" s="43" t="s">
         <v>68</v>
       </c>
@@ -8103,27 +8095,27 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="19.5" thickBot="1">
+    <row r="62" spans="1:1" ht="19" thickBot="1">
       <c r="A62" s="46" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="15.75" thickBot="1">
+    <row r="63" spans="1:1" ht="15" thickBot="1">
       <c r="A63" s="45" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="15.75" thickBot="1">
+    <row r="64" spans="1:1" ht="15" thickBot="1">
       <c r="A64" s="43" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="15.75" thickBot="1">
+    <row r="65" spans="1:1" ht="15" thickBot="1">
       <c r="A65" s="43" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="15.75" thickBot="1">
+    <row r="66" spans="1:1" ht="15" thickBot="1">
       <c r="A66" s="43" t="s">
         <v>75</v>
       </c>
@@ -8133,17 +8125,17 @@
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="15.75" thickBot="1">
+    <row r="68" spans="1:1" ht="15" thickBot="1">
       <c r="A68" s="44" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="15.75" thickBot="1">
+    <row r="69" spans="1:1" ht="15" thickBot="1">
       <c r="A69" s="43" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="15.75" thickBot="1">
+    <row r="70" spans="1:1" ht="15" thickBot="1">
       <c r="A70" s="43" t="s">
         <v>79</v>
       </c>
@@ -8153,62 +8145,62 @@
         <v>80</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="15.75" thickBot="1">
+    <row r="72" spans="1:1" ht="15" thickBot="1">
       <c r="A72" s="44" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="15.75" thickBot="1">
+    <row r="73" spans="1:1" ht="15" thickBot="1">
       <c r="A73" s="43" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="15.75" thickBot="1">
+    <row r="74" spans="1:1" ht="15" thickBot="1">
       <c r="A74" s="43" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="15.75" thickBot="1">
+    <row r="75" spans="1:1" ht="15" thickBot="1">
       <c r="A75" s="43" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="15.75" thickBot="1">
+    <row r="76" spans="1:1" ht="15" thickBot="1">
       <c r="A76" s="43" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="15.75" thickBot="1">
+    <row r="77" spans="1:1" ht="15" thickBot="1">
       <c r="A77" s="43" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="15.75" thickBot="1">
+    <row r="78" spans="1:1" ht="15" thickBot="1">
       <c r="A78" s="43" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="15.75" thickBot="1">
+    <row r="79" spans="1:1" ht="15" thickBot="1">
       <c r="A79" s="43" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="15.75" thickBot="1">
+    <row r="80" spans="1:1" ht="15" thickBot="1">
       <c r="A80" s="43" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="15.75" thickBot="1">
+    <row r="81" spans="1:1" ht="15" thickBot="1">
       <c r="A81" s="43" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="15.75" thickBot="1">
+    <row r="82" spans="1:1" ht="15" thickBot="1">
       <c r="A82" s="43" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="15.75" thickBot="1">
+    <row r="83" spans="1:1" ht="15" thickBot="1">
       <c r="A83" s="43" t="s">
         <v>92</v>
       </c>
@@ -8218,12 +8210,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="15.75" thickBot="1">
+    <row r="85" spans="1:1" ht="15" thickBot="1">
       <c r="A85" s="44" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="15.75" thickBot="1">
+    <row r="86" spans="1:1" ht="15" thickBot="1">
       <c r="A86" s="43" t="s">
         <v>94</v>
       </c>
@@ -8238,122 +8230,122 @@
         <v>96</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="19.5" thickBot="1">
+    <row r="89" spans="1:1" ht="19" thickBot="1">
       <c r="A89" s="46" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="15.75" thickBot="1">
+    <row r="90" spans="1:1" ht="15" thickBot="1">
       <c r="A90" s="45" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="15.75" thickBot="1">
+    <row r="91" spans="1:1" ht="15" thickBot="1">
       <c r="A91" s="43" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="15.75" thickBot="1">
+    <row r="92" spans="1:1" ht="15" thickBot="1">
       <c r="A92" s="43" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="15.75" thickBot="1">
+    <row r="93" spans="1:1" ht="15" thickBot="1">
       <c r="A93" s="43" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="15.75" thickBot="1">
+    <row r="94" spans="1:1" ht="15" thickBot="1">
       <c r="A94" s="43" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="15.75" thickBot="1">
+    <row r="95" spans="1:1" ht="15" thickBot="1">
       <c r="A95" s="43" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:1" ht="15.75" thickBot="1">
+    <row r="96" spans="1:1" ht="15" thickBot="1">
       <c r="A96" s="43" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="97" spans="1:1" ht="15.75" thickBot="1">
+    <row r="97" spans="1:1" ht="15" thickBot="1">
       <c r="A97" s="43" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="1:1" ht="15.75" thickBot="1">
+    <row r="98" spans="1:1" ht="15" thickBot="1">
       <c r="A98" s="43" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="99" spans="1:1" ht="15.75" thickBot="1">
+    <row r="99" spans="1:1" ht="15" thickBot="1">
       <c r="A99" s="43" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="100" spans="1:1" ht="15.75" thickBot="1">
+    <row r="100" spans="1:1" ht="15" thickBot="1">
       <c r="A100" s="43" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="101" spans="1:1" ht="15.75" thickBot="1">
+    <row r="101" spans="1:1" ht="15" thickBot="1">
       <c r="A101" s="43" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="102" spans="1:1" ht="15.75" thickBot="1">
+    <row r="102" spans="1:1" ht="15" thickBot="1">
       <c r="A102" s="43" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="103" spans="1:1" ht="15.75" thickBot="1">
+    <row r="103" spans="1:1" ht="15" thickBot="1">
       <c r="A103" s="43" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="104" spans="1:1" ht="15.75" thickBot="1">
+    <row r="104" spans="1:1" ht="15" thickBot="1">
       <c r="A104" s="43" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="105" spans="1:1" ht="15.75" thickBot="1">
+    <row r="105" spans="1:1" ht="15" thickBot="1">
       <c r="A105" s="43" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="15.75" thickBot="1">
+    <row r="106" spans="1:1" ht="15" thickBot="1">
       <c r="A106" s="43" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="107" spans="1:1" ht="15.75" thickBot="1">
+    <row r="107" spans="1:1" ht="15" thickBot="1">
       <c r="A107" s="43" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="108" spans="1:1" ht="15.75" thickBot="1">
+    <row r="108" spans="1:1" ht="15" thickBot="1">
       <c r="A108" s="43" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="109" spans="1:1" ht="15.75" thickBot="1">
+    <row r="109" spans="1:1" ht="15" thickBot="1">
       <c r="A109" s="43" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="110" spans="1:1" ht="15.75" thickBot="1">
+    <row r="110" spans="1:1" ht="15" thickBot="1">
       <c r="A110" s="43" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="111" spans="1:1" ht="15.75" thickBot="1">
+    <row r="111" spans="1:1" ht="15" thickBot="1">
       <c r="A111" s="43" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="112" spans="1:1" ht="15.75" thickBot="1">
+    <row r="112" spans="1:1" ht="15" thickBot="1">
       <c r="A112" s="43" t="s">
         <v>120</v>
       </c>
@@ -8368,72 +8360,72 @@
         <v>122</v>
       </c>
     </row>
-    <row r="115" spans="1:1" ht="19.5" thickBot="1">
+    <row r="115" spans="1:1" ht="19" thickBot="1">
       <c r="A115" s="46" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="116" spans="1:1" ht="15.75" thickBot="1">
+    <row r="116" spans="1:1" ht="15" thickBot="1">
       <c r="A116" s="45" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="117" spans="1:1" ht="15.75" thickBot="1">
+    <row r="117" spans="1:1" ht="15" thickBot="1">
       <c r="A117" s="43" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="118" spans="1:1" ht="15.75" thickBot="1">
+    <row r="118" spans="1:1" ht="15" thickBot="1">
       <c r="A118" s="43" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="119" spans="1:1" ht="15.75" thickBot="1">
+    <row r="119" spans="1:1" ht="15" thickBot="1">
       <c r="A119" s="43" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="120" spans="1:1" ht="15.75" thickBot="1">
+    <row r="120" spans="1:1" ht="15" thickBot="1">
       <c r="A120" s="43" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="121" spans="1:1" ht="15.75" thickBot="1">
+    <row r="121" spans="1:1" ht="15" thickBot="1">
       <c r="A121" s="43" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="122" spans="1:1" ht="15.75" thickBot="1">
+    <row r="122" spans="1:1" ht="15" thickBot="1">
       <c r="A122" s="43" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="123" spans="1:1" ht="15.75" thickBot="1">
+    <row r="123" spans="1:1" ht="15" thickBot="1">
       <c r="A123" s="43" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="124" spans="1:1" ht="15.75" thickBot="1">
+    <row r="124" spans="1:1" ht="15" thickBot="1">
       <c r="A124" s="43" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="125" spans="1:1" ht="15.75" thickBot="1">
+    <row r="125" spans="1:1" ht="15" thickBot="1">
       <c r="A125" s="43" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="126" spans="1:1" ht="15.75" thickBot="1">
+    <row r="126" spans="1:1" ht="15" thickBot="1">
       <c r="A126" s="43" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="127" spans="1:1" ht="15.75" thickBot="1">
+    <row r="127" spans="1:1" ht="15" thickBot="1">
       <c r="A127" s="43" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="128" spans="1:1" ht="15.75" thickBot="1">
+    <row r="128" spans="1:1" ht="15" thickBot="1">
       <c r="A128" s="43" t="s">
         <v>136</v>
       </c>
@@ -8448,87 +8440,87 @@
         <v>138</v>
       </c>
     </row>
-    <row r="131" spans="1:1" ht="19.5" thickBot="1">
+    <row r="131" spans="1:1" ht="19" thickBot="1">
       <c r="A131" s="46" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="132" spans="1:1" ht="15.75" thickBot="1">
+    <row r="132" spans="1:1" ht="15" thickBot="1">
       <c r="A132" s="45" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="133" spans="1:1" ht="15.75" thickBot="1">
+    <row r="133" spans="1:1" ht="15" thickBot="1">
       <c r="A133" s="43" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="134" spans="1:1" ht="15.75" thickBot="1">
+    <row r="134" spans="1:1" ht="15" thickBot="1">
       <c r="A134" s="43" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="135" spans="1:1" ht="15.75" thickBot="1">
+    <row r="135" spans="1:1" ht="15" thickBot="1">
       <c r="A135" s="43" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="136" spans="1:1" ht="15.75" thickBot="1">
+    <row r="136" spans="1:1" ht="15" thickBot="1">
       <c r="A136" s="43" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="137" spans="1:1" ht="15.75" thickBot="1">
+    <row r="137" spans="1:1" ht="15" thickBot="1">
       <c r="A137" s="43" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="138" spans="1:1" ht="15.75" thickBot="1">
+    <row r="138" spans="1:1" ht="15" thickBot="1">
       <c r="A138" s="43" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="139" spans="1:1" ht="15.75" thickBot="1">
+    <row r="139" spans="1:1" ht="15" thickBot="1">
       <c r="A139" s="43" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="140" spans="1:1" ht="15.75" thickBot="1">
+    <row r="140" spans="1:1" ht="15" thickBot="1">
       <c r="A140" s="43" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="141" spans="1:1" ht="15.75" thickBot="1">
+    <row r="141" spans="1:1" ht="15" thickBot="1">
       <c r="A141" s="43" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="142" spans="1:1" ht="15.75" thickBot="1">
+    <row r="142" spans="1:1" ht="15" thickBot="1">
       <c r="A142" s="43" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="143" spans="1:1" ht="15.75" thickBot="1">
+    <row r="143" spans="1:1" ht="15" thickBot="1">
       <c r="A143" s="43" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="144" spans="1:1" ht="15.75" thickBot="1">
+    <row r="144" spans="1:1" ht="15" thickBot="1">
       <c r="A144" s="43" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="145" spans="1:1" ht="15.75" thickBot="1">
+    <row r="145" spans="1:1" ht="15" thickBot="1">
       <c r="A145" s="43" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="146" spans="1:1" ht="15.75" thickBot="1">
+    <row r="146" spans="1:1" ht="15" thickBot="1">
       <c r="A146" s="43" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="147" spans="1:1" ht="15.75" thickBot="1">
+    <row r="147" spans="1:1" ht="15" thickBot="1">
       <c r="A147" s="43" t="s">
         <v>155</v>
       </c>
@@ -8543,17 +8535,17 @@
         <v>157</v>
       </c>
     </row>
-    <row r="150" spans="1:1" ht="19.5" thickBot="1">
+    <row r="150" spans="1:1" ht="19" thickBot="1">
       <c r="A150" s="46" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="151" spans="1:1" ht="15.75" thickBot="1">
+    <row r="151" spans="1:1" ht="15" thickBot="1">
       <c r="A151" s="45" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="152" spans="1:1" ht="15.75" thickBot="1">
+    <row r="152" spans="1:1" ht="15" thickBot="1">
       <c r="A152" s="43" t="s">
         <v>160</v>
       </c>
@@ -8563,7 +8555,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="154" spans="1:1" ht="15.75" thickBot="1">
+    <row r="154" spans="1:1" ht="15" thickBot="1">
       <c r="A154" s="44" t="s">
         <v>162</v>
       </c>
@@ -8573,7 +8565,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="156" spans="1:1" ht="15.75" thickBot="1">
+    <row r="156" spans="1:1" ht="15" thickBot="1">
       <c r="A156" s="44" t="s">
         <v>164</v>
       </c>
@@ -8583,17 +8575,17 @@
         <v>165</v>
       </c>
     </row>
-    <row r="158" spans="1:1" ht="15.75" thickBot="1">
+    <row r="158" spans="1:1" ht="15" thickBot="1">
       <c r="A158" s="44" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="159" spans="1:1" ht="15.75" thickBot="1">
+    <row r="159" spans="1:1" ht="15" thickBot="1">
       <c r="A159" s="43" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="160" spans="1:1" ht="15.75" thickBot="1">
+    <row r="160" spans="1:1" ht="15" thickBot="1">
       <c r="A160" s="43" t="s">
         <v>168</v>
       </c>
@@ -8603,102 +8595,102 @@
         <v>169</v>
       </c>
     </row>
-    <row r="162" spans="1:1" ht="15.75" thickBot="1">
+    <row r="162" spans="1:1" ht="15" thickBot="1">
       <c r="A162" s="44" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="163" spans="1:1" ht="15.75" thickBot="1">
+    <row r="163" spans="1:1" ht="15" thickBot="1">
       <c r="A163" s="43" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="164" spans="1:1" ht="15.75" thickBot="1">
+    <row r="164" spans="1:1" ht="15" thickBot="1">
       <c r="A164" s="43" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="165" spans="1:1" ht="15.75" thickBot="1">
+    <row r="165" spans="1:1" ht="15" thickBot="1">
       <c r="A165" s="43" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="166" spans="1:1" ht="15.75" thickBot="1">
+    <row r="166" spans="1:1" ht="15" thickBot="1">
       <c r="A166" s="43" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="167" spans="1:1" ht="15.75" thickBot="1">
+    <row r="167" spans="1:1" ht="15" thickBot="1">
       <c r="A167" s="43" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="168" spans="1:1" ht="15.75" thickBot="1">
+    <row r="168" spans="1:1" ht="15" thickBot="1">
       <c r="A168" s="43" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="169" spans="1:1" ht="15.75" thickBot="1">
+    <row r="169" spans="1:1" ht="15" thickBot="1">
       <c r="A169" s="43" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="170" spans="1:1" ht="15.75" thickBot="1">
+    <row r="170" spans="1:1" ht="15" thickBot="1">
       <c r="A170" s="43" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="171" spans="1:1" ht="15.75" thickBot="1">
+    <row r="171" spans="1:1" ht="15" thickBot="1">
       <c r="A171" s="43" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="172" spans="1:1" ht="15.75" thickBot="1">
+    <row r="172" spans="1:1" ht="15" thickBot="1">
       <c r="A172" s="43" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="173" spans="1:1" ht="15.75" thickBot="1">
+    <row r="173" spans="1:1" ht="15" thickBot="1">
       <c r="A173" s="43" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="174" spans="1:1" ht="15.75" thickBot="1">
+    <row r="174" spans="1:1" ht="15" thickBot="1">
       <c r="A174" s="43" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="175" spans="1:1" ht="15.75" thickBot="1">
+    <row r="175" spans="1:1" ht="15" thickBot="1">
       <c r="A175" s="43" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="176" spans="1:1" ht="15.75" thickBot="1">
+    <row r="176" spans="1:1" ht="15" thickBot="1">
       <c r="A176" s="43" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="177" spans="1:1" ht="15.75" thickBot="1">
+    <row r="177" spans="1:1" ht="15" thickBot="1">
       <c r="A177" s="43" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="178" spans="1:1" ht="15.75" thickBot="1">
+    <row r="178" spans="1:1" ht="15" thickBot="1">
       <c r="A178" s="43" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="179" spans="1:1" ht="15.75" thickBot="1">
+    <row r="179" spans="1:1" ht="15" thickBot="1">
       <c r="A179" s="43" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="180" spans="1:1" ht="15.75" thickBot="1">
+    <row r="180" spans="1:1" ht="15" thickBot="1">
       <c r="A180" s="43" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="181" spans="1:1" ht="15.75" thickBot="1">
+    <row r="181" spans="1:1" ht="15" thickBot="1">
       <c r="A181" s="43" t="s">
         <v>189</v>
       </c>
@@ -8708,22 +8700,22 @@
         <v>190</v>
       </c>
     </row>
-    <row r="183" spans="1:1" ht="15.75" thickBot="1">
+    <row r="183" spans="1:1" ht="15" thickBot="1">
       <c r="A183" s="44" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="184" spans="1:1" ht="15.75" thickBot="1">
+    <row r="184" spans="1:1" ht="15" thickBot="1">
       <c r="A184" s="43" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="185" spans="1:1" ht="15.75" thickBot="1">
+    <row r="185" spans="1:1" ht="15" thickBot="1">
       <c r="A185" s="43" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="186" spans="1:1" ht="15.75" thickBot="1">
+    <row r="186" spans="1:1" ht="15" thickBot="1">
       <c r="A186" s="43" t="s">
         <v>194</v>
       </c>
@@ -8733,32 +8725,32 @@
         <v>195</v>
       </c>
     </row>
-    <row r="188" spans="1:1" ht="15.75" thickBot="1">
+    <row r="188" spans="1:1" ht="15" thickBot="1">
       <c r="A188" s="44" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="189" spans="1:1" ht="15.75" thickBot="1">
+    <row r="189" spans="1:1" ht="15" thickBot="1">
       <c r="A189" s="43" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="190" spans="1:1" ht="15.75" thickBot="1">
+    <row r="190" spans="1:1" ht="15" thickBot="1">
       <c r="A190" s="43" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="191" spans="1:1" ht="15.75" thickBot="1">
+    <row r="191" spans="1:1" ht="15" thickBot="1">
       <c r="A191" s="43" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="192" spans="1:1" ht="15.75" thickBot="1">
+    <row r="192" spans="1:1" ht="15" thickBot="1">
       <c r="A192" s="43" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="193" spans="1:1" ht="15.75" thickBot="1">
+    <row r="193" spans="1:1" ht="15" thickBot="1">
       <c r="A193" s="43" t="s">
         <v>201</v>
       </c>
@@ -8773,87 +8765,87 @@
         <v>203</v>
       </c>
     </row>
-    <row r="196" spans="1:1" ht="19.5" thickBot="1">
+    <row r="196" spans="1:1" ht="19" thickBot="1">
       <c r="A196" s="46" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="197" spans="1:1" ht="15.75" thickBot="1">
+    <row r="197" spans="1:1" ht="15" thickBot="1">
       <c r="A197" s="45" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="198" spans="1:1" ht="15.75" thickBot="1">
+    <row r="198" spans="1:1" ht="15" thickBot="1">
       <c r="A198" s="43" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="199" spans="1:1" ht="15.75" thickBot="1">
+    <row r="199" spans="1:1" ht="15" thickBot="1">
       <c r="A199" s="43" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="200" spans="1:1" ht="15.75" thickBot="1">
+    <row r="200" spans="1:1" ht="15" thickBot="1">
       <c r="A200" s="43" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="201" spans="1:1" ht="15.75" thickBot="1">
+    <row r="201" spans="1:1" ht="15" thickBot="1">
       <c r="A201" s="43" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="202" spans="1:1" ht="15.75" thickBot="1">
+    <row r="202" spans="1:1" ht="15" thickBot="1">
       <c r="A202" s="43" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="203" spans="1:1" ht="15.75" thickBot="1">
+    <row r="203" spans="1:1" ht="15" thickBot="1">
       <c r="A203" s="43" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="204" spans="1:1" ht="15.75" thickBot="1">
+    <row r="204" spans="1:1" ht="15" thickBot="1">
       <c r="A204" s="43" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="205" spans="1:1" ht="15.75" thickBot="1">
+    <row r="205" spans="1:1" ht="15" thickBot="1">
       <c r="A205" s="43" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="206" spans="1:1" ht="15.75" thickBot="1">
+    <row r="206" spans="1:1" ht="15" thickBot="1">
       <c r="A206" s="43" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="207" spans="1:1" ht="15.75" thickBot="1">
+    <row r="207" spans="1:1" ht="15" thickBot="1">
       <c r="A207" s="43" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="208" spans="1:1" ht="15.75" thickBot="1">
+    <row r="208" spans="1:1" ht="15" thickBot="1">
       <c r="A208" s="43" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="209" spans="1:1" ht="15.75" thickBot="1">
+    <row r="209" spans="1:1" ht="15" thickBot="1">
       <c r="A209" s="43" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="210" spans="1:1" ht="15.75" thickBot="1">
+    <row r="210" spans="1:1" ht="15" thickBot="1">
       <c r="A210" s="43" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="211" spans="1:1" ht="15.75" thickBot="1">
+    <row r="211" spans="1:1" ht="15" thickBot="1">
       <c r="A211" s="43" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="212" spans="1:1" ht="15.75" thickBot="1">
+    <row r="212" spans="1:1" ht="15" thickBot="1">
       <c r="A212" s="43" t="s">
         <v>220</v>
       </c>
@@ -8868,22 +8860,22 @@
         <v>222</v>
       </c>
     </row>
-    <row r="215" spans="1:1" ht="19.5" thickBot="1">
+    <row r="215" spans="1:1" ht="19" thickBot="1">
       <c r="A215" s="46" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="216" spans="1:1" ht="15.75" thickBot="1">
+    <row r="216" spans="1:1" ht="15" thickBot="1">
       <c r="A216" s="43" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="217" spans="1:1" ht="15.75" thickBot="1">
+    <row r="217" spans="1:1" ht="15" thickBot="1">
       <c r="A217" s="43" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="218" spans="1:1" ht="15.75" thickBot="1">
+    <row r="218" spans="1:1" ht="15" thickBot="1">
       <c r="A218" s="43" t="s">
         <v>226</v>
       </c>
@@ -8895,6 +8887,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more progress on excel vba course
</commit_message>
<xml_diff>
--- a/Ultimate Excel Programmer - VBA (Udemy) - Video Listing.xlsx
+++ b/Ultimate Excel Programmer - VBA (Udemy) - Video Listing.xlsx
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="252">
   <si>
     <t>VIDEO NAME</t>
   </si>
@@ -1133,6 +1133,9 @@
   </si>
   <si>
     <t>on hold until after Unity exam</t>
+  </si>
+  <si>
+    <t>59. Relative Positioning using Offset  4:13</t>
   </si>
 </sst>
 </file>
@@ -1469,9 +1472,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="38">
+  <cellStyleXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1638,7 +1643,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="38">
+  <cellStyles count="40">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -1657,6 +1662,7 @@
     <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1675,6 +1681,7 @@
     <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1981,8 +1988,8 @@
   <dimension ref="A1:K198"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G71" sqref="G71"/>
+      <pane ySplit="3" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" outlineLevelRow="1" x14ac:dyDescent="0"/>
@@ -2010,7 +2017,7 @@
       </c>
       <c r="F1" s="34">
         <f>SUMIF(G4:G196, "&gt;0", C4:C196)</f>
-        <v>181</v>
+        <v>191</v>
       </c>
       <c r="G1" s="35">
         <f>+C197</f>
@@ -2018,7 +2025,7 @@
       </c>
       <c r="H1" s="36">
         <f>+F1/G1</f>
-        <v>0.26346433770014555</v>
+        <v>0.27802037845705968</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -4140,8 +4147,12 @@
         <f t="shared" si="6"/>
         <v>0.26783114992721996</v>
       </c>
-      <c r="G71" s="30"/>
-      <c r="H71" s="30"/>
+      <c r="G71" s="30">
+        <v>42921</v>
+      </c>
+      <c r="H71" s="30">
+        <v>42921</v>
+      </c>
       <c r="I71" s="9" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -4167,8 +4178,12 @@
         <f t="shared" ref="F72:F135" si="14">F71+(C72/$C$197)</f>
         <v>0.27802037845705985</v>
       </c>
-      <c r="G72" s="30"/>
-      <c r="H72" s="30"/>
+      <c r="G72" s="30">
+        <v>42921</v>
+      </c>
+      <c r="H72" s="30">
+        <v>42921</v>
+      </c>
       <c r="I72" s="9" t="str">
         <f t="shared" ref="I72:I135" si="15">IF(H72="", "", IF(ISBLANK(H73), IF(H72&lt;&gt;H74, SUMIF(H:H,H72,C:C), ""), IF(H72&lt;&gt;H73, SUMIF(H:H,H72,C:C), "")))</f>
         <v/>
@@ -4180,7 +4195,7 @@
     </row>
     <row r="73" spans="1:10" outlineLevel="1">
       <c r="B73" s="18" t="s">
-        <v>92</v>
+        <v>251</v>
       </c>
       <c r="C73" s="13">
         <v>4</v>
@@ -4195,7 +4210,9 @@
         <v>0.28384279475982549</v>
       </c>
       <c r="G73" s="30"/>
-      <c r="H73" s="30"/>
+      <c r="H73" s="30">
+        <v>42921</v>
+      </c>
       <c r="I73" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4222,7 +4239,9 @@
         <v>0.29112081513828253</v>
       </c>
       <c r="G74" s="30"/>
-      <c r="H74" s="30"/>
+      <c r="H74" s="30">
+        <v>42921</v>
+      </c>
       <c r="I74" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4249,7 +4268,9 @@
         <v>0.32751091703056784</v>
       </c>
       <c r="G75" s="30"/>
-      <c r="H75" s="30"/>
+      <c r="H75" s="30">
+        <v>42921</v>
+      </c>
       <c r="I75" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4276,14 +4297,16 @@
         <v>0.33478893740902488</v>
       </c>
       <c r="G76" s="30"/>
-      <c r="H76" s="30"/>
-      <c r="I76" s="9" t="str">
+      <c r="H76" s="30">
+        <v>42921</v>
+      </c>
+      <c r="I76" s="9">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="J76" s="38" t="str">
+        <v>49</v>
+      </c>
+      <c r="J76" s="38">
         <f t="shared" si="16"/>
-        <v/>
+        <v>0.81666666666666665</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="21" thickBot="1">
@@ -4335,15 +4358,15 @@
       </c>
       <c r="G78" s="30"/>
       <c r="H78" s="30">
-        <v>42897</v>
-      </c>
-      <c r="I78" s="9" t="str">
+        <v>42922</v>
+      </c>
+      <c r="I78" s="9">
         <f t="shared" si="15"/>
-        <v/>
-      </c>
-      <c r="J78" s="38" t="str">
+        <v>3</v>
+      </c>
+      <c r="J78" s="38">
         <f t="shared" si="16"/>
-        <v/>
+        <v>0.05</v>
       </c>
     </row>
     <row r="79" spans="1:10" outlineLevel="1">
@@ -4363,9 +4386,7 @@
         <v>0.34497816593886477</v>
       </c>
       <c r="G79" s="30"/>
-      <c r="H79" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H79" s="30"/>
       <c r="I79" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4392,9 +4413,7 @@
         <v>0.35371179039301326</v>
       </c>
       <c r="G80" s="30"/>
-      <c r="H80" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H80" s="30"/>
       <c r="I80" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4421,9 +4440,7 @@
         <v>0.3580786026200875</v>
       </c>
       <c r="G81" s="30"/>
-      <c r="H81" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H81" s="30"/>
       <c r="I81" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4450,9 +4467,7 @@
         <v>0.36244541484716175</v>
       </c>
       <c r="G82" s="30"/>
-      <c r="H82" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H82" s="30"/>
       <c r="I82" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4479,9 +4494,7 @@
         <v>0.366812227074236</v>
       </c>
       <c r="G83" s="30"/>
-      <c r="H83" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H83" s="30"/>
       <c r="I83" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4508,9 +4521,7 @@
         <v>0.36972343522561885</v>
       </c>
       <c r="G84" s="30"/>
-      <c r="H84" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H84" s="30"/>
       <c r="I84" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4537,9 +4548,7 @@
         <v>0.37700145560407589</v>
       </c>
       <c r="G85" s="30"/>
-      <c r="H85" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H85" s="30"/>
       <c r="I85" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4566,9 +4575,7 @@
         <v>0.38719068413391577</v>
       </c>
       <c r="G86" s="30"/>
-      <c r="H86" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H86" s="30"/>
       <c r="I86" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4595,9 +4602,7 @@
         <v>0.39301310043668142</v>
       </c>
       <c r="G87" s="30"/>
-      <c r="H87" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H87" s="30"/>
       <c r="I87" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4624,9 +4629,7 @@
         <v>0.39883551673944706</v>
       </c>
       <c r="G88" s="30"/>
-      <c r="H88" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H88" s="30"/>
       <c r="I88" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4653,9 +4656,7 @@
         <v>0.40029112081513846</v>
       </c>
       <c r="G89" s="30"/>
-      <c r="H89" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H89" s="30"/>
       <c r="I89" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4682,9 +4683,7 @@
         <v>0.40320232896652131</v>
       </c>
       <c r="G90" s="30"/>
-      <c r="H90" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H90" s="30"/>
       <c r="I90" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4711,9 +4710,7 @@
         <v>0.40611353711790416</v>
       </c>
       <c r="G91" s="30"/>
-      <c r="H91" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H91" s="30"/>
       <c r="I91" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4740,9 +4737,7 @@
         <v>0.4104803493449784</v>
       </c>
       <c r="G92" s="30"/>
-      <c r="H92" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H92" s="30"/>
       <c r="I92" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4769,9 +4764,7 @@
         <v>0.41775836972343544</v>
       </c>
       <c r="G93" s="30"/>
-      <c r="H93" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H93" s="30"/>
       <c r="I93" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4798,9 +4791,7 @@
         <v>0.42358078602620108</v>
       </c>
       <c r="G94" s="30"/>
-      <c r="H94" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H94" s="30"/>
       <c r="I94" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4827,9 +4818,7 @@
         <v>0.42940320232896673</v>
       </c>
       <c r="G95" s="30"/>
-      <c r="H95" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H95" s="30"/>
       <c r="I95" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4856,9 +4845,7 @@
         <v>0.43231441048034958</v>
       </c>
       <c r="G96" s="30"/>
-      <c r="H96" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H96" s="30"/>
       <c r="I96" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4885,9 +4872,7 @@
         <v>0.43522561863173242</v>
       </c>
       <c r="G97" s="30"/>
-      <c r="H97" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H97" s="30"/>
       <c r="I97" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4914,9 +4899,7 @@
         <v>0.43813682678311527</v>
       </c>
       <c r="G98" s="30"/>
-      <c r="H98" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H98" s="30"/>
       <c r="I98" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4943,9 +4926,7 @@
         <v>0.43959243085880667</v>
       </c>
       <c r="G99" s="30"/>
-      <c r="H99" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H99" s="30"/>
       <c r="I99" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -4972,9 +4953,7 @@
         <v>0.44250363901018952</v>
       </c>
       <c r="G100" s="30"/>
-      <c r="H100" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H100" s="30"/>
       <c r="I100" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5001,9 +4980,7 @@
         <v>0.44978165938864656</v>
       </c>
       <c r="G101" s="30"/>
-      <c r="H101" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H101" s="30"/>
       <c r="I101" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5061,9 +5038,7 @@
         <v>0.4556040756914122</v>
       </c>
       <c r="G103" s="30"/>
-      <c r="H103" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H103" s="30"/>
       <c r="I103" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5090,9 +5065,7 @@
         <v>0.45851528384279505</v>
       </c>
       <c r="G104" s="30"/>
-      <c r="H104" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H104" s="30"/>
       <c r="I104" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5119,9 +5092,7 @@
         <v>0.4628820960698693</v>
       </c>
       <c r="G105" s="30"/>
-      <c r="H105" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H105" s="30"/>
       <c r="I105" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5148,9 +5119,7 @@
         <v>0.46433770014556069</v>
       </c>
       <c r="G106" s="30"/>
-      <c r="H106" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H106" s="30"/>
       <c r="I106" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5177,9 +5146,7 @@
         <v>0.46870451237263494</v>
       </c>
       <c r="G107" s="30"/>
-      <c r="H107" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H107" s="30"/>
       <c r="I107" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5206,9 +5173,7 @@
         <v>0.47161572052401779</v>
       </c>
       <c r="G108" s="30"/>
-      <c r="H108" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H108" s="30"/>
       <c r="I108" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5235,9 +5200,7 @@
         <v>0.47598253275109204</v>
       </c>
       <c r="G109" s="30"/>
-      <c r="H109" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H109" s="30"/>
       <c r="I109" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5264,9 +5227,7 @@
         <v>0.47889374090247488</v>
       </c>
       <c r="G110" s="30"/>
-      <c r="H110" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H110" s="30"/>
       <c r="I110" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5293,9 +5254,7 @@
         <v>0.48034934497816628</v>
       </c>
       <c r="G111" s="30"/>
-      <c r="H111" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H111" s="30"/>
       <c r="I111" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5322,9 +5281,7 @@
         <v>0.48762736535662332</v>
       </c>
       <c r="G112" s="30"/>
-      <c r="H112" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H112" s="30"/>
       <c r="I112" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5351,9 +5308,7 @@
         <v>0.49199417758369757</v>
       </c>
       <c r="G113" s="30"/>
-      <c r="H113" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H113" s="30"/>
       <c r="I113" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5380,9 +5335,7 @@
         <v>0.49636098981077181</v>
       </c>
       <c r="G114" s="30"/>
-      <c r="H114" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H114" s="30"/>
       <c r="I114" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5409,9 +5362,7 @@
         <v>0.50072780203784606</v>
       </c>
       <c r="G115" s="30"/>
-      <c r="H115" s="30">
-        <v>42897</v>
-      </c>
+      <c r="H115" s="30"/>
       <c r="I115" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5438,16 +5389,14 @@
         <v>0.5080058224163031</v>
       </c>
       <c r="G116" s="30"/>
-      <c r="H116" s="30">
-        <v>42897</v>
-      </c>
-      <c r="I116" s="9">
+      <c r="H116" s="30"/>
+      <c r="I116" s="9" t="str">
         <f t="shared" si="15"/>
-        <v>119</v>
-      </c>
-      <c r="J116" s="38">
+        <v/>
+      </c>
+      <c r="J116" s="38" t="str">
         <f t="shared" si="16"/>
-        <v>1.9833333333333334</v>
+        <v/>
       </c>
     </row>
     <row r="117" spans="1:10" ht="21" thickBot="1">
@@ -5498,9 +5447,7 @@
         <v>0.51528384279476014</v>
       </c>
       <c r="G118" s="30"/>
-      <c r="H118" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H118" s="30"/>
       <c r="I118" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5527,9 +5474,7 @@
         <v>0.51819505094614293</v>
       </c>
       <c r="G119" s="30"/>
-      <c r="H119" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H119" s="30"/>
       <c r="I119" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5556,9 +5501,7 @@
         <v>0.52256186317321718</v>
       </c>
       <c r="G120" s="30"/>
-      <c r="H120" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H120" s="30"/>
       <c r="I120" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5585,9 +5528,7 @@
         <v>0.52547307132459997</v>
       </c>
       <c r="G121" s="30"/>
-      <c r="H121" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H121" s="30"/>
       <c r="I121" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5614,9 +5555,7 @@
         <v>0.53129548762736567</v>
       </c>
       <c r="G122" s="30"/>
-      <c r="H122" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H122" s="30"/>
       <c r="I122" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5643,9 +5582,7 @@
         <v>0.53420669577874846</v>
       </c>
       <c r="G123" s="30"/>
-      <c r="H123" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H123" s="30"/>
       <c r="I123" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5672,9 +5609,7 @@
         <v>0.53566229985443992</v>
       </c>
       <c r="G124" s="30"/>
-      <c r="H124" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H124" s="30"/>
       <c r="I124" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5701,9 +5636,7 @@
         <v>0.54002911208151416</v>
       </c>
       <c r="G125" s="30"/>
-      <c r="H125" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H125" s="30"/>
       <c r="I125" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5730,9 +5663,7 @@
         <v>0.54294032023289696</v>
       </c>
       <c r="G126" s="30"/>
-      <c r="H126" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H126" s="30"/>
       <c r="I126" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5759,9 +5690,7 @@
         <v>0.54585152838427975</v>
       </c>
       <c r="G127" s="30"/>
-      <c r="H127" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H127" s="30"/>
       <c r="I127" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5788,9 +5717,7 @@
         <v>0.55312954876273679</v>
       </c>
       <c r="G128" s="30"/>
-      <c r="H128" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H128" s="30"/>
       <c r="I128" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5817,9 +5744,7 @@
         <v>0.55749636098981104</v>
       </c>
       <c r="G129" s="30"/>
-      <c r="H129" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H129" s="30"/>
       <c r="I129" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5846,9 +5771,7 @@
         <v>0.55895196506550249</v>
       </c>
       <c r="G130" s="30"/>
-      <c r="H130" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H130" s="30"/>
       <c r="I130" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5875,9 +5798,7 @@
         <v>0.56040756914119394</v>
       </c>
       <c r="G131" s="30"/>
-      <c r="H131" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H131" s="30"/>
       <c r="I131" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5904,9 +5825,7 @@
         <v>0.56186317321688539</v>
       </c>
       <c r="G132" s="30"/>
-      <c r="H132" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H132" s="30"/>
       <c r="I132" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5933,9 +5852,7 @@
         <v>0.56331877729257684</v>
       </c>
       <c r="G133" s="30"/>
-      <c r="H133" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H133" s="30"/>
       <c r="I133" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -5962,9 +5879,7 @@
         <v>0.56622998544395964</v>
       </c>
       <c r="G134" s="30"/>
-      <c r="H134" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H134" s="30"/>
       <c r="I134" s="9" t="str">
         <f t="shared" si="15"/>
         <v/>
@@ -6022,9 +5937,7 @@
         <v>0.57205240174672534</v>
       </c>
       <c r="G136" s="30"/>
-      <c r="H136" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H136" s="30"/>
       <c r="I136" s="9" t="str">
         <f t="shared" ref="I136:I195" si="22">IF(H136="", "", IF(ISBLANK(H137), IF(H136&lt;&gt;H138, SUMIF(H:H,H136,C:C), ""), IF(H136&lt;&gt;H137, SUMIF(H:H,H136,C:C), "")))</f>
         <v/>
@@ -6051,9 +5964,7 @@
         <v>0.57787481804949103</v>
       </c>
       <c r="G137" s="30"/>
-      <c r="H137" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H137" s="30"/>
       <c r="I137" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6080,9 +5991,7 @@
         <v>0.58369723435225673</v>
       </c>
       <c r="G138" s="30"/>
-      <c r="H138" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H138" s="30"/>
       <c r="I138" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6109,9 +6018,7 @@
         <v>0.58951965065502243</v>
       </c>
       <c r="G139" s="30"/>
-      <c r="H139" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H139" s="30"/>
       <c r="I139" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6138,9 +6045,7 @@
         <v>0.59388646288209668</v>
       </c>
       <c r="G140" s="30"/>
-      <c r="H140" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H140" s="30"/>
       <c r="I140" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6167,9 +6072,7 @@
         <v>0.59679767103347947</v>
       </c>
       <c r="G141" s="30"/>
-      <c r="H141" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H141" s="30"/>
       <c r="I141" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6196,9 +6099,7 @@
         <v>0.60262008733624517</v>
       </c>
       <c r="G142" s="30"/>
-      <c r="H142" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H142" s="30"/>
       <c r="I142" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6225,9 +6126,7 @@
         <v>0.612809315866085</v>
       </c>
       <c r="G143" s="30"/>
-      <c r="H143" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H143" s="30"/>
       <c r="I143" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6254,9 +6153,7 @@
         <v>0.61426491994177645</v>
       </c>
       <c r="G144" s="30"/>
-      <c r="H144" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H144" s="30"/>
       <c r="I144" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6283,9 +6180,7 @@
         <v>0.6186317321688507</v>
       </c>
       <c r="G145" s="30"/>
-      <c r="H145" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H145" s="30"/>
       <c r="I145" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6312,9 +6207,7 @@
         <v>0.62154294032023349</v>
       </c>
       <c r="G146" s="30"/>
-      <c r="H146" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H146" s="30"/>
       <c r="I146" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6341,9 +6234,7 @@
         <v>0.62445414847161629</v>
       </c>
       <c r="G147" s="30"/>
-      <c r="H147" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H147" s="30"/>
       <c r="I147" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6370,9 +6261,7 @@
         <v>0.62882096069869053</v>
       </c>
       <c r="G148" s="30"/>
-      <c r="H148" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H148" s="30"/>
       <c r="I148" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6399,9 +6288,7 @@
         <v>0.63318777292576478</v>
       </c>
       <c r="G149" s="30"/>
-      <c r="H149" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H149" s="30"/>
       <c r="I149" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6428,9 +6315,7 @@
         <v>0.64046579330422182</v>
       </c>
       <c r="G150" s="30"/>
-      <c r="H150" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H150" s="30"/>
       <c r="I150" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6457,9 +6342,7 @@
         <v>0.64628820960698752</v>
       </c>
       <c r="G151" s="30"/>
-      <c r="H151" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H151" s="30"/>
       <c r="I151" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6486,9 +6369,7 @@
         <v>0.6608442503639016</v>
       </c>
       <c r="G152" s="30"/>
-      <c r="H152" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H152" s="30"/>
       <c r="I152" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6515,9 +6396,7 @@
         <v>0.66812227074235864</v>
       </c>
       <c r="G153" s="30"/>
-      <c r="H153" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H153" s="30"/>
       <c r="I153" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6544,9 +6423,7 @@
         <v>0.67685589519650713</v>
       </c>
       <c r="G154" s="30"/>
-      <c r="H154" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H154" s="30"/>
       <c r="I154" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6573,9 +6450,7 @@
         <v>0.68267831149927283</v>
       </c>
       <c r="G155" s="30"/>
-      <c r="H155" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H155" s="30"/>
       <c r="I155" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6602,9 +6477,7 @@
         <v>0.68850072780203853</v>
       </c>
       <c r="G156" s="30"/>
-      <c r="H156" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H156" s="30"/>
       <c r="I156" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6631,9 +6504,7 @@
         <v>0.69432314410480422</v>
       </c>
       <c r="G157" s="30"/>
-      <c r="H157" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H157" s="30"/>
       <c r="I157" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6660,9 +6531,7 @@
         <v>0.70014556040756992</v>
       </c>
       <c r="G158" s="30"/>
-      <c r="H158" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H158" s="30"/>
       <c r="I158" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6689,9 +6558,7 @@
         <v>0.70742358078602696</v>
       </c>
       <c r="G159" s="30"/>
-      <c r="H159" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H159" s="30"/>
       <c r="I159" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6718,9 +6585,7 @@
         <v>0.71179039301310121</v>
       </c>
       <c r="G160" s="30"/>
-      <c r="H160" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H160" s="30"/>
       <c r="I160" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6747,9 +6612,7 @@
         <v>0.72634643377001529</v>
       </c>
       <c r="G161" s="30"/>
-      <c r="H161" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H161" s="30"/>
       <c r="I161" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6776,9 +6639,7 @@
         <v>0.73508005822416378</v>
       </c>
       <c r="G162" s="30"/>
-      <c r="H162" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H162" s="30"/>
       <c r="I162" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6805,9 +6666,7 @@
         <v>0.74526928675400361</v>
       </c>
       <c r="G163" s="30"/>
-      <c r="H163" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H163" s="30"/>
       <c r="I163" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6834,9 +6693,7 @@
         <v>0.7569141193595349</v>
       </c>
       <c r="G164" s="30"/>
-      <c r="H164" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H164" s="30"/>
       <c r="I164" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6863,9 +6720,7 @@
         <v>0.7627365356623006</v>
       </c>
       <c r="G165" s="30"/>
-      <c r="H165" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H165" s="30"/>
       <c r="I165" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6892,9 +6747,7 @@
         <v>0.77147016011644909</v>
       </c>
       <c r="G166" s="30"/>
-      <c r="H166" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H166" s="30"/>
       <c r="I166" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6921,9 +6774,7 @@
         <v>0.77729257641921479</v>
       </c>
       <c r="G167" s="30"/>
-      <c r="H167" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H167" s="30"/>
       <c r="I167" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6950,9 +6801,7 @@
         <v>0.79184861717612887</v>
       </c>
       <c r="G168" s="30"/>
-      <c r="H168" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H168" s="30"/>
       <c r="I168" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -6979,9 +6828,7 @@
         <v>0.79767103347889456</v>
       </c>
       <c r="G169" s="30"/>
-      <c r="H169" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H169" s="30"/>
       <c r="I169" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7008,9 +6855,7 @@
         <v>0.80349344978166026</v>
       </c>
       <c r="G170" s="30"/>
-      <c r="H170" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H170" s="30"/>
       <c r="I170" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7037,9 +6882,7 @@
         <v>0.81222707423580875</v>
       </c>
       <c r="G171" s="30"/>
-      <c r="H171" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H171" s="30"/>
       <c r="I171" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7066,9 +6909,7 @@
         <v>0.816593886462883</v>
       </c>
       <c r="G172" s="30"/>
-      <c r="H172" s="30">
-        <v>42898</v>
-      </c>
+      <c r="H172" s="30"/>
       <c r="I172" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7095,16 +6936,14 @@
         <v>0.81950509461426579</v>
       </c>
       <c r="G173" s="30"/>
-      <c r="H173" s="30">
-        <v>42898</v>
-      </c>
-      <c r="I173" s="9">
+      <c r="H173" s="30"/>
+      <c r="I173" s="9" t="str">
         <f t="shared" si="22"/>
-        <v>214</v>
-      </c>
-      <c r="J173" s="38">
+        <v/>
+      </c>
+      <c r="J173" s="38" t="str">
         <f t="shared" si="23"/>
-        <v>3.5666666666666669</v>
+        <v/>
       </c>
     </row>
     <row r="174" spans="1:10" ht="21" thickBot="1">
@@ -7155,9 +6994,7 @@
         <v>0.82823871906841429</v>
       </c>
       <c r="G175" s="30"/>
-      <c r="H175" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H175" s="30"/>
       <c r="I175" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7184,9 +7021,7 @@
         <v>0.83842794759825412</v>
       </c>
       <c r="G176" s="30"/>
-      <c r="H176" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H176" s="30"/>
       <c r="I176" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7213,9 +7048,7 @@
         <v>0.84425036390101982</v>
       </c>
       <c r="G177" s="30"/>
-      <c r="H177" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H177" s="30"/>
       <c r="I177" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7242,9 +7075,7 @@
         <v>0.85735080058224256</v>
       </c>
       <c r="G178" s="30"/>
-      <c r="H178" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H178" s="30"/>
       <c r="I178" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7271,9 +7102,7 @@
         <v>0.8617176128093168</v>
       </c>
       <c r="G179" s="30"/>
-      <c r="H179" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H179" s="30"/>
       <c r="I179" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7300,9 +7129,7 @@
         <v>0.8646288209606996</v>
       </c>
       <c r="G180" s="30"/>
-      <c r="H180" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H180" s="30"/>
       <c r="I180" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7329,9 +7156,7 @@
         <v>0.86899563318777384</v>
       </c>
       <c r="G181" s="30"/>
-      <c r="H181" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H181" s="30"/>
       <c r="I181" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7358,9 +7183,7 @@
         <v>0.87772925764192233</v>
       </c>
       <c r="G182" s="30"/>
-      <c r="H182" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H182" s="30"/>
       <c r="I182" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7387,9 +7210,7 @@
         <v>0.89519650655021932</v>
       </c>
       <c r="G183" s="30"/>
-      <c r="H183" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H183" s="30"/>
       <c r="I183" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7416,9 +7237,7 @@
         <v>0.9068413391557506</v>
       </c>
       <c r="G184" s="30"/>
-      <c r="H184" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H184" s="30"/>
       <c r="I184" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7445,9 +7264,7 @@
         <v>0.93013100436681317</v>
       </c>
       <c r="G185" s="30"/>
-      <c r="H185" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H185" s="30"/>
       <c r="I185" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7474,9 +7291,7 @@
         <v>0.94614264919941871</v>
       </c>
       <c r="G186" s="30"/>
-      <c r="H186" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H186" s="30"/>
       <c r="I186" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7503,9 +7318,7 @@
         <v>0.9548762736535672</v>
       </c>
       <c r="G187" s="30"/>
-      <c r="H187" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H187" s="30"/>
       <c r="I187" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7532,9 +7345,7 @@
         <v>0.95924308588064144</v>
       </c>
       <c r="G188" s="30"/>
-      <c r="H188" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H188" s="30"/>
       <c r="I188" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7561,9 +7372,7 @@
         <v>0.96360989810771569</v>
       </c>
       <c r="G189" s="30"/>
-      <c r="H189" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H189" s="30"/>
       <c r="I189" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7590,9 +7399,7 @@
         <v>0.97234352256186418</v>
       </c>
       <c r="G190" s="30"/>
-      <c r="H190" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H190" s="30"/>
       <c r="I190" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7619,9 +7426,7 @@
         <v>0.97671033478893843</v>
       </c>
       <c r="G191" s="30"/>
-      <c r="H191" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H191" s="30"/>
       <c r="I191" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7679,9 +7484,7 @@
         <v>0.98689956331877826</v>
       </c>
       <c r="G193" s="30"/>
-      <c r="H193" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H193" s="30"/>
       <c r="I193" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7708,9 +7511,7 @@
         <v>0.99563318777292675</v>
       </c>
       <c r="G194" s="30"/>
-      <c r="H194" s="30">
-        <v>42899</v>
-      </c>
+      <c r="H194" s="30"/>
       <c r="I194" s="9" t="str">
         <f t="shared" si="22"/>
         <v/>
@@ -7737,16 +7538,14 @@
         <v>1.0000000000000009</v>
       </c>
       <c r="G195" s="30"/>
-      <c r="H195" s="30">
-        <v>42899</v>
-      </c>
-      <c r="I195" s="9">
+      <c r="H195" s="30"/>
+      <c r="I195" s="9" t="str">
         <f t="shared" si="22"/>
-        <v>124</v>
-      </c>
-      <c r="J195" s="38">
+        <v/>
+      </c>
+      <c r="J195" s="38" t="str">
         <f t="shared" si="23"/>
-        <v>2.0666666666666669</v>
+        <v/>
       </c>
     </row>
     <row r="197" spans="2:10" ht="15" thickBot="1">

</xml_diff>